<commit_message>
:updated odds and fixtures
</commit_message>
<xml_diff>
--- a/spreadex.xlsx
+++ b/spreadex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kovan\FDAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BCD331-4095-4A81-B518-D2887E67501F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78735124-B5E0-4EEA-BC53-F09CF2A4DB0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="802" xr2:uid="{8365F371-5EDF-4C19-B0B3-71E11A5B2E12}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3872" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4100" uniqueCount="761">
   <si>
     <t>24/11/2022 20:55</t>
   </si>
@@ -2144,6 +2144,189 @@
   </si>
   <si>
     <t>16/02/2023 17:42</t>
+  </si>
+  <si>
+    <t>24/02/2023 19:31</t>
+  </si>
+  <si>
+    <t>Mainz v M'Gladbach</t>
+  </si>
+  <si>
+    <t>24/02/2023 19:29</t>
+  </si>
+  <si>
+    <t>Karlsruhe v Jahn Regensburg</t>
+  </si>
+  <si>
+    <t>24/02/2023 19:11</t>
+  </si>
+  <si>
+    <t>Sparta Rotterdam v Utrecht</t>
+  </si>
+  <si>
+    <t>24/02/2023 17:35</t>
+  </si>
+  <si>
+    <t>24/02/2023 17:29</t>
+  </si>
+  <si>
+    <t>23/02/2023 21:53</t>
+  </si>
+  <si>
+    <t>Man Utd v Barcelona</t>
+  </si>
+  <si>
+    <t>23/02/2023 20:13</t>
+  </si>
+  <si>
+    <t>22/02/2023 21:58</t>
+  </si>
+  <si>
+    <t>Inter Milan v Porto</t>
+  </si>
+  <si>
+    <t>22/02/2023 21:53</t>
+  </si>
+  <si>
+    <t>RB Leipzig v Man City</t>
+  </si>
+  <si>
+    <t>22/02/2023 21:38</t>
+  </si>
+  <si>
+    <t>22/02/2023 20:33</t>
+  </si>
+  <si>
+    <t>22/02/2023 20:08</t>
+  </si>
+  <si>
+    <t>22/02/2023 20:01</t>
+  </si>
+  <si>
+    <t>Real Betis v Real Madrid</t>
+  </si>
+  <si>
+    <t>Liverpool v Man Utd</t>
+  </si>
+  <si>
+    <t>Leverkusen v Hertha BSC</t>
+  </si>
+  <si>
+    <t>Fiorentina v AC Milan</t>
+  </si>
+  <si>
+    <t>Boavista v Arouca</t>
+  </si>
+  <si>
+    <t>Napoli v Lazio</t>
+  </si>
+  <si>
+    <t>Dortmund v RB Leipzig</t>
+  </si>
+  <si>
+    <t>Magdeburg v Kaiserslautern</t>
+  </si>
+  <si>
+    <t>Alanyaspor v Basaksehir</t>
+  </si>
+  <si>
+    <t>Real Madrid v Barcelona</t>
+  </si>
+  <si>
+    <t>Liverpool v Wolves</t>
+  </si>
+  <si>
+    <t>27/02/2023 19:13</t>
+  </si>
+  <si>
+    <t>Sporting Lisbon v Estoril</t>
+  </si>
+  <si>
+    <t>27/02/2023 19:03</t>
+  </si>
+  <si>
+    <t>26/02/2023 21:37</t>
+  </si>
+  <si>
+    <t>Marseille v Paris Saint-Germain</t>
+  </si>
+  <si>
+    <t>26/02/2023 19:31</t>
+  </si>
+  <si>
+    <t>26/02/2023 14:21</t>
+  </si>
+  <si>
+    <t>Tottenham v Chelsea</t>
+  </si>
+  <si>
+    <t>26/02/2023 13:57</t>
+  </si>
+  <si>
+    <t>26/02/2023 13:02</t>
+  </si>
+  <si>
+    <t>Arminia Bielefeld v Heidenheim</t>
+  </si>
+  <si>
+    <t>26/02/2023 12:27</t>
+  </si>
+  <si>
+    <t>25/02/2023 19:28</t>
+  </si>
+  <si>
+    <t>Real Madrid v Atletico Madrid</t>
+  </si>
+  <si>
+    <t>25/02/2023 17:36</t>
+  </si>
+  <si>
+    <t>25/02/2023 15:45</t>
+  </si>
+  <si>
+    <t>Birmingham v Luton</t>
+  </si>
+  <si>
+    <t>25/02/2023 14:53</t>
+  </si>
+  <si>
+    <t>Espanyol v Mallorca</t>
+  </si>
+  <si>
+    <t>25/02/2023 14:39</t>
+  </si>
+  <si>
+    <t>Hoffenheim v Dortmund</t>
+  </si>
+  <si>
+    <t>25/02/2023 14:31</t>
+  </si>
+  <si>
+    <t>25/02/2023 13:54</t>
+  </si>
+  <si>
+    <t>Holstein Kiel v Paderborn</t>
+  </si>
+  <si>
+    <t>25/02/2023 13:17</t>
+  </si>
+  <si>
+    <t>25/02/2023 12:02</t>
+  </si>
+  <si>
+    <t>24/02/2023 21:58</t>
+  </si>
+  <si>
+    <t>Fulham v Wolves</t>
+  </si>
+  <si>
+    <t>24/02/2023 21:26</t>
+  </si>
+  <si>
+    <t>24/02/2023 21:07</t>
+  </si>
+  <si>
+    <t>24/02/2023 20:29</t>
   </si>
 </sst>
 </file>
@@ -2704,13 +2887,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B2ACDE7-BC8B-432A-9773-10E95E9E94B1}">
-  <dimension ref="A1:V1083"/>
+  <dimension ref="A1:V1150"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B1075" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B1099" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I1097" sqref="I1097"/>
+      <selection pane="bottomRight" activeCell="A1110" sqref="A1110:G1110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20792,7 +20975,7 @@
       <c r="G1071" s="3"/>
     </row>
     <row r="1072" spans="1:7" ht="15.75" thickBot="1"/>
-    <row r="1073" spans="1:7" ht="15.75" thickBot="1">
+    <row r="1073" spans="1:19" ht="15.75" thickBot="1">
       <c r="A1073" s="2" t="s">
         <v>641</v>
       </c>
@@ -20815,7 +20998,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="1074" spans="1:7" ht="15.75" thickBot="1">
+    <row r="1074" spans="1:19" ht="15.75" thickBot="1">
       <c r="A1074" s="2" t="s">
         <v>642</v>
       </c>
@@ -20836,8 +21019,8 @@
       </c>
       <c r="G1074" s="3"/>
     </row>
-    <row r="1075" spans="1:7" ht="15.75" thickBot="1"/>
-    <row r="1076" spans="1:7" ht="15.75" thickBot="1">
+    <row r="1075" spans="1:19" ht="15.75" thickBot="1"/>
+    <row r="1076" spans="1:19" ht="15.75" thickBot="1">
       <c r="A1076" s="2" t="s">
         <v>636</v>
       </c>
@@ -20860,7 +21043,7 @@
         <v>-0.52</v>
       </c>
     </row>
-    <row r="1077" spans="1:7" ht="15.75" thickBot="1">
+    <row r="1077" spans="1:19" ht="15.75" thickBot="1">
       <c r="A1077" s="2" t="s">
         <v>638</v>
       </c>
@@ -20881,8 +21064,8 @@
       </c>
       <c r="G1077" s="3"/>
     </row>
-    <row r="1078" spans="1:7" ht="15.75" thickBot="1"/>
-    <row r="1079" spans="1:7" ht="15.75" thickBot="1">
+    <row r="1078" spans="1:19" ht="15.75" thickBot="1"/>
+    <row r="1079" spans="1:19" ht="15.75" thickBot="1">
       <c r="A1079" s="2" t="s">
         <v>633</v>
       </c>
@@ -20905,7 +21088,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="1080" spans="1:7" ht="15.75" thickBot="1">
+    <row r="1080" spans="1:19" ht="15.75" thickBot="1">
       <c r="A1080" s="2" t="s">
         <v>635</v>
       </c>
@@ -20926,8 +21109,8 @@
       </c>
       <c r="G1080" s="3"/>
     </row>
-    <row r="1081" spans="1:7" ht="15.75" thickBot="1"/>
-    <row r="1082" spans="1:7" ht="15.75" thickBot="1">
+    <row r="1081" spans="1:19" ht="15.75" thickBot="1"/>
+    <row r="1082" spans="1:19" ht="15.75" thickBot="1">
       <c r="A1082" s="2" t="s">
         <v>630</v>
       </c>
@@ -20950,7 +21133,7 @@
         <v>-0.12</v>
       </c>
     </row>
-    <row r="1083" spans="1:7" ht="15.75" thickBot="1">
+    <row r="1083" spans="1:19" ht="15.75" thickBot="1">
       <c r="A1083" s="2" t="s">
         <v>632</v>
       </c>
@@ -20970,6 +21153,1499 @@
         <v>5</v>
       </c>
       <c r="G1083" s="3"/>
+    </row>
+    <row r="1084" spans="1:19" ht="15.75" thickBot="1">
+      <c r="L1084" s="1"/>
+      <c r="M1084" s="1"/>
+      <c r="N1084" s="1"/>
+      <c r="O1084" s="1"/>
+      <c r="P1084" s="1"/>
+      <c r="Q1084" s="1"/>
+      <c r="R1084" s="1"/>
+      <c r="S1084" s="1"/>
+    </row>
+    <row r="1085" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A1085" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="B1085" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1085" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="D1085" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1085" s="4">
+        <v>69</v>
+      </c>
+      <c r="F1085" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1085" s="5">
+        <v>0.26</v>
+      </c>
+      <c r="S1085" s="2"/>
+    </row>
+    <row r="1086" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A1086" s="2" t="s">
+        <v>716</v>
+      </c>
+      <c r="B1086" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1086" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="D1086" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1086" s="4">
+        <v>43</v>
+      </c>
+      <c r="F1086" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1086" s="3"/>
+      <c r="S1086" s="2"/>
+    </row>
+    <row r="1087" spans="1:19" ht="15.75" thickBot="1">
+      <c r="S1087" s="2"/>
+    </row>
+    <row r="1088" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A1088" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="B1088" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1088" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="D1088" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1088" s="4">
+        <v>36</v>
+      </c>
+      <c r="F1088" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1088" s="3">
+        <v>-0.71</v>
+      </c>
+      <c r="S1088" s="2"/>
+    </row>
+    <row r="1089" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A1089" s="2" t="s">
+        <v>718</v>
+      </c>
+      <c r="B1089" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1089" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="D1089" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1089" s="4">
+        <v>107</v>
+      </c>
+      <c r="F1089" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1089" s="3"/>
+      <c r="R1089" s="3"/>
+      <c r="S1089" s="2"/>
+    </row>
+    <row r="1090" spans="1:19" ht="15.75" thickBot="1">
+      <c r="S1090" s="2"/>
+    </row>
+    <row r="1091" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A1091" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="B1091" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1091" s="2" t="s">
+        <v>714</v>
+      </c>
+      <c r="D1091" s="3">
+        <v>-0.18</v>
+      </c>
+      <c r="E1091" s="4">
+        <v>2</v>
+      </c>
+      <c r="F1091" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1091" s="3">
+        <v>-0.12</v>
+      </c>
+      <c r="S1091" s="2"/>
+    </row>
+    <row r="1092" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A1092" s="2" t="s">
+        <v>717</v>
+      </c>
+      <c r="B1092" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1092" s="2" t="s">
+        <v>714</v>
+      </c>
+      <c r="D1092" s="5">
+        <v>0.18</v>
+      </c>
+      <c r="E1092" s="4">
+        <v>2.65</v>
+      </c>
+      <c r="F1092" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1092" s="3"/>
+      <c r="S1092" s="2"/>
+    </row>
+    <row r="1093" spans="1:19" ht="15.75" thickBot="1">
+      <c r="S1093" s="2"/>
+    </row>
+    <row r="1094" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A1094" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="B1094" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1094" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="D1094" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1094" s="4">
+        <v>60</v>
+      </c>
+      <c r="F1094" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1094" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="S1094" s="2"/>
+    </row>
+    <row r="1095" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A1095" s="2" t="s">
+        <v>710</v>
+      </c>
+      <c r="B1095" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1095" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="D1095" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1095" s="4">
+        <v>50</v>
+      </c>
+      <c r="F1095" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1095" s="3"/>
+      <c r="S1095" s="2"/>
+    </row>
+    <row r="1096" spans="1:19" ht="15.75" thickBot="1">
+      <c r="S1096" s="2"/>
+    </row>
+    <row r="1097" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A1097" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="B1097" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1097" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="D1097" s="3">
+        <v>-0.18</v>
+      </c>
+      <c r="E1097" s="4">
+        <v>1</v>
+      </c>
+      <c r="F1097" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1097" s="3">
+        <v>-0.34</v>
+      </c>
+      <c r="S1097" s="2"/>
+    </row>
+    <row r="1098" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A1098" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="B1098" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1098" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="D1098" s="5">
+        <v>0.18</v>
+      </c>
+      <c r="E1098" s="4">
+        <v>2.9</v>
+      </c>
+      <c r="F1098" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1098" s="3"/>
+      <c r="S1098" s="2"/>
+    </row>
+    <row r="1099" spans="1:19" ht="15.75" thickBot="1"/>
+    <row r="1100" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A1100" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="B1100" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1100" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="D1100" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1100" s="4">
+        <v>36</v>
+      </c>
+      <c r="F1100" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1100" s="3">
+        <v>-0.75</v>
+      </c>
+      <c r="L1100" s="1"/>
+      <c r="M1100" s="1"/>
+      <c r="N1100" s="1"/>
+      <c r="O1100" s="1"/>
+      <c r="P1100" s="1"/>
+      <c r="Q1100" s="1"/>
+      <c r="R1100" s="1"/>
+      <c r="S1100" s="1"/>
+    </row>
+    <row r="1101" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A1101" s="2" t="s">
+        <v>706</v>
+      </c>
+      <c r="B1101" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1101" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="D1101" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1101" s="4">
+        <v>111</v>
+      </c>
+      <c r="F1101" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1101" s="11">
+        <v>45049.912499999999</v>
+      </c>
+      <c r="M1101" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N1101" s="2" t="s">
+        <v>719</v>
+      </c>
+      <c r="O1101" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="P1101" s="4">
+        <v>64</v>
+      </c>
+      <c r="Q1101" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1101" s="3">
+        <v>-0.47</v>
+      </c>
+      <c r="S1101" s="2"/>
+    </row>
+    <row r="1102" spans="1:19" ht="15.75" thickBot="1">
+      <c r="L1102" s="11">
+        <v>45049.82916666667</v>
+      </c>
+      <c r="M1102" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N1102" s="2" t="s">
+        <v>719</v>
+      </c>
+      <c r="O1102" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="P1102" s="4">
+        <v>111</v>
+      </c>
+      <c r="Q1102" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1102" s="3"/>
+      <c r="S1102" s="2"/>
+    </row>
+    <row r="1103" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A1103" s="2" t="s">
+        <v>759</v>
+      </c>
+      <c r="B1103" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1103" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="D1103" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1103" s="4">
+        <v>36</v>
+      </c>
+      <c r="F1103" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1103" s="3">
+        <v>-0.56999999999999995</v>
+      </c>
+      <c r="L1103" s="11">
+        <v>45049.746527777781</v>
+      </c>
+      <c r="M1103" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1103" s="2" t="s">
+        <v>720</v>
+      </c>
+      <c r="O1103" s="3">
+        <v>-0.02</v>
+      </c>
+      <c r="P1103" s="4">
+        <v>60</v>
+      </c>
+      <c r="Q1103" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1103" s="5">
+        <v>0.18</v>
+      </c>
+      <c r="S1103" s="2"/>
+    </row>
+    <row r="1104" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A1104" s="2" t="s">
+        <v>704</v>
+      </c>
+      <c r="B1104" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1104" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="D1104" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1104" s="4">
+        <v>93</v>
+      </c>
+      <c r="F1104" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1104" s="3"/>
+      <c r="L1104" s="11">
+        <v>45049.688888888886</v>
+      </c>
+      <c r="M1104" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1104" s="2" t="s">
+        <v>720</v>
+      </c>
+      <c r="O1104" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="P1104" s="4">
+        <v>51</v>
+      </c>
+      <c r="Q1104" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1104" s="3"/>
+      <c r="S1104" s="2"/>
+    </row>
+    <row r="1105" spans="1:19" ht="15.75" thickBot="1">
+      <c r="L1105" s="11">
+        <v>45049.613888888889</v>
+      </c>
+      <c r="M1105" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N1105" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="O1105" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="P1105" s="4">
+        <v>117</v>
+      </c>
+      <c r="Q1105" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1105" s="5">
+        <v>0.18</v>
+      </c>
+      <c r="S1105" s="2"/>
+    </row>
+    <row r="1106" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A1106" s="2" t="s">
+        <v>758</v>
+      </c>
+      <c r="B1106" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1106" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="D1106" s="3">
+        <v>-0.18</v>
+      </c>
+      <c r="E1106" s="4">
+        <v>4</v>
+      </c>
+      <c r="F1106" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1106" s="5">
+        <v>0.18</v>
+      </c>
+      <c r="L1106" s="11">
+        <v>45049.602777777778</v>
+      </c>
+      <c r="M1106" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N1106" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="O1106" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="P1106" s="4">
+        <v>99</v>
+      </c>
+      <c r="Q1106" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1106" s="3"/>
+      <c r="S1106" s="2"/>
+    </row>
+    <row r="1107" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A1107" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="B1107" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1107" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="D1107" s="5">
+        <v>0.18</v>
+      </c>
+      <c r="E1107" s="4">
+        <v>3</v>
+      </c>
+      <c r="F1107" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1107" s="3"/>
+      <c r="L1107" s="11">
+        <v>45019.904861111114</v>
+      </c>
+      <c r="M1107" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1107" s="2" t="s">
+        <v>722</v>
+      </c>
+      <c r="O1107" s="3">
+        <v>-0.2</v>
+      </c>
+      <c r="P1107" s="4">
+        <v>3</v>
+      </c>
+      <c r="Q1107" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1107" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="S1107" s="2"/>
+    </row>
+    <row r="1108" spans="1:19" ht="15.75" thickBot="1">
+      <c r="L1108" s="11">
+        <v>45019.840277777781</v>
+      </c>
+      <c r="M1108" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1108" s="2" t="s">
+        <v>722</v>
+      </c>
+      <c r="O1108" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="P1108" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q1108" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1108" s="3"/>
+      <c r="S1108" s="2"/>
+    </row>
+    <row r="1109" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A1109" s="2" t="s">
+        <v>756</v>
+      </c>
+      <c r="B1109" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1109" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="D1109" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1109" s="4">
+        <v>20</v>
+      </c>
+      <c r="F1109" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1109" s="3">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="L1109" s="11">
+        <v>45019.835416666669</v>
+      </c>
+      <c r="M1109" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N1109" s="2" t="s">
+        <v>722</v>
+      </c>
+      <c r="O1109" s="3">
+        <v>-0.02</v>
+      </c>
+      <c r="P1109" s="4">
+        <v>167</v>
+      </c>
+      <c r="Q1109" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1109" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="S1109" s="2"/>
+    </row>
+    <row r="1110" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A1110" s="2" t="s">
+        <v>760</v>
+      </c>
+      <c r="B1110" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1110" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="D1110" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1110" s="4">
+        <v>48</v>
+      </c>
+      <c r="F1110" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1110" s="3"/>
+      <c r="L1110" s="11">
+        <v>45019.809027777781</v>
+      </c>
+      <c r="M1110" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N1110" s="2" t="s">
+        <v>722</v>
+      </c>
+      <c r="O1110" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="P1110" s="4">
+        <v>102</v>
+      </c>
+      <c r="Q1110" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1110" s="3"/>
+      <c r="S1110" s="2"/>
+    </row>
+    <row r="1111" spans="1:19" ht="15.75" thickBot="1">
+      <c r="L1111" s="11">
+        <v>44988.959027777775</v>
+      </c>
+      <c r="M1111" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N1111" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="O1111" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="P1111" s="4">
+        <v>49</v>
+      </c>
+      <c r="Q1111" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1111" s="3">
+        <v>-0.76</v>
+      </c>
+      <c r="S1111" s="2"/>
+    </row>
+    <row r="1112" spans="1:19" ht="15.75" thickBot="1">
+      <c r="L1112" s="11">
+        <v>44988.900694444441</v>
+      </c>
+      <c r="M1112" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1112" s="2" t="s">
+        <v>724</v>
+      </c>
+      <c r="O1112" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="P1112" s="4">
+        <v>40</v>
+      </c>
+      <c r="Q1112" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1112" s="3">
+        <v>-0.12</v>
+      </c>
+      <c r="S1112" s="2"/>
+    </row>
+    <row r="1113" spans="1:19" ht="15.75" thickBot="1">
+      <c r="L1113" s="11">
+        <v>44988.893055555556</v>
+      </c>
+      <c r="M1113" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N1113" s="2" t="s">
+        <v>725</v>
+      </c>
+      <c r="O1113" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="P1113" s="4">
+        <v>100</v>
+      </c>
+      <c r="Q1113" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1113" s="3">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="S1113" s="2"/>
+    </row>
+    <row r="1114" spans="1:19" ht="15.75" thickBot="1">
+      <c r="L1114" s="11">
+        <v>44988.831944444442</v>
+      </c>
+      <c r="M1114" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1114" s="2" t="s">
+        <v>724</v>
+      </c>
+      <c r="O1114" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="P1114" s="4">
+        <v>52</v>
+      </c>
+      <c r="Q1114" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1114" s="3"/>
+      <c r="S1114" s="2"/>
+    </row>
+    <row r="1115" spans="1:19" ht="15.75" thickBot="1">
+      <c r="L1115" s="11">
+        <v>44988.813194444447</v>
+      </c>
+      <c r="M1115" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N1115" s="2" t="s">
+        <v>725</v>
+      </c>
+      <c r="O1115" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="P1115" s="4">
+        <v>107</v>
+      </c>
+      <c r="Q1115" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1115" s="3"/>
+      <c r="S1115" s="2"/>
+    </row>
+    <row r="1116" spans="1:19" ht="15.75" thickBot="1">
+      <c r="L1116" s="11">
+        <v>44988.79791666667</v>
+      </c>
+      <c r="M1116" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N1116" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="O1116" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="P1116" s="4">
+        <v>125</v>
+      </c>
+      <c r="Q1116" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1116" s="3"/>
+      <c r="S1116" s="2"/>
+    </row>
+    <row r="1117" spans="1:19" ht="15.75" thickBot="1">
+      <c r="L1117" s="11">
+        <v>44988.792361111111</v>
+      </c>
+      <c r="M1117" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1117" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="O1117" s="3">
+        <v>-0.18</v>
+      </c>
+      <c r="P1117" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="Q1117" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1117" s="5">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S1117" s="2"/>
+    </row>
+    <row r="1118" spans="1:19" ht="15.75" thickBot="1">
+      <c r="L1118" s="11">
+        <v>44988.789583333331</v>
+      </c>
+      <c r="M1118" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N1118" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="O1118" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="P1118" s="4">
+        <v>123</v>
+      </c>
+      <c r="Q1118" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1118" s="5">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S1118" s="2"/>
+    </row>
+    <row r="1119" spans="1:19" ht="15.75" thickBot="1">
+      <c r="L1119" s="11">
+        <v>44988.756944444445</v>
+      </c>
+      <c r="M1119" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1119" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="O1119" s="5">
+        <v>0.18</v>
+      </c>
+      <c r="P1119" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="Q1119" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1119" s="3"/>
+      <c r="S1119" s="2"/>
+    </row>
+    <row r="1120" spans="1:19" ht="15.75" thickBot="1">
+      <c r="L1120" s="11">
+        <v>44988.753472222219</v>
+      </c>
+      <c r="M1120" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N1120" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="O1120" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="P1120" s="4">
+        <v>113</v>
+      </c>
+      <c r="Q1120" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1120" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="S1120" s="2"/>
+    </row>
+    <row r="1121" spans="12:19" ht="15.75" thickBot="1">
+      <c r="L1121" s="11">
+        <v>44988.729861111111</v>
+      </c>
+      <c r="M1121" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N1121" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="O1121" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="P1121" s="4">
+        <v>112</v>
+      </c>
+      <c r="Q1121" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1121" s="3"/>
+      <c r="S1121" s="2"/>
+    </row>
+    <row r="1122" spans="12:19" ht="15.75" thickBot="1">
+      <c r="L1122" s="11">
+        <v>44988.706944444442</v>
+      </c>
+      <c r="M1122" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N1122" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="O1122" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="P1122" s="4">
+        <v>109</v>
+      </c>
+      <c r="Q1122" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1122" s="3"/>
+      <c r="S1122" s="2"/>
+    </row>
+    <row r="1123" spans="12:19" ht="15.75" thickBot="1">
+      <c r="L1123" s="11">
+        <v>44960.9</v>
+      </c>
+      <c r="M1123" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1123" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="O1123" s="3">
+        <v>-0.02</v>
+      </c>
+      <c r="P1123" s="4">
+        <v>77</v>
+      </c>
+      <c r="Q1123" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1123" s="5">
+        <v>0.44</v>
+      </c>
+      <c r="S1123" s="2"/>
+    </row>
+    <row r="1124" spans="12:19" ht="15.75" thickBot="1">
+      <c r="L1124" s="11">
+        <v>44960.881249999999</v>
+      </c>
+      <c r="M1124" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N1124" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="O1124" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="P1124" s="4">
+        <v>132</v>
+      </c>
+      <c r="Q1124" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1124" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="S1124" s="2"/>
+    </row>
+    <row r="1125" spans="12:19" ht="15.75" thickBot="1">
+      <c r="L1125" s="11">
+        <v>44960.848611111112</v>
+      </c>
+      <c r="M1125" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1125" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="O1125" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="P1125" s="4">
+        <v>55</v>
+      </c>
+      <c r="Q1125" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1125" s="3"/>
+      <c r="S1125" s="2"/>
+    </row>
+    <row r="1126" spans="12:19" ht="15.75" thickBot="1">
+      <c r="L1126" s="11">
+        <v>44960.834722222222</v>
+      </c>
+      <c r="M1126" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N1126" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="O1126" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="P1126" s="4">
+        <v>104</v>
+      </c>
+      <c r="Q1126" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1126" s="3"/>
+      <c r="S1126" s="2"/>
+    </row>
+    <row r="1127" spans="12:19" ht="15.75" thickBot="1">
+      <c r="L1127" s="11">
+        <v>44929.884027777778</v>
+      </c>
+      <c r="M1127" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1127" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="O1127" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="P1127" s="4">
+        <v>59</v>
+      </c>
+      <c r="Q1127" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1127" s="5">
+        <v>0.24</v>
+      </c>
+      <c r="S1127" s="2"/>
+    </row>
+    <row r="1128" spans="12:19" ht="15.75" thickBot="1">
+      <c r="L1128" s="11">
+        <v>44929.839583333334</v>
+      </c>
+      <c r="M1128" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1128" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="O1128" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="P1128" s="4">
+        <v>35</v>
+      </c>
+      <c r="Q1128" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1128" s="3"/>
+      <c r="S1128" s="2"/>
+    </row>
+    <row r="1129" spans="12:19" ht="15.75" thickBot="1">
+      <c r="L1129" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="M1129" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N1129" s="2" t="s">
+        <v>731</v>
+      </c>
+      <c r="O1129" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="P1129" s="4">
+        <v>180</v>
+      </c>
+      <c r="Q1129" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1129" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="S1129" s="2"/>
+    </row>
+    <row r="1130" spans="12:19" ht="15.75" thickBot="1">
+      <c r="L1130" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="M1130" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N1130" s="2" t="s">
+        <v>731</v>
+      </c>
+      <c r="O1130" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="P1130" s="4">
+        <v>120</v>
+      </c>
+      <c r="Q1130" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1130" s="3"/>
+      <c r="S1130" s="2"/>
+    </row>
+    <row r="1131" spans="12:19" ht="15.75" thickBot="1">
+      <c r="L1131" s="2" t="s">
+        <v>733</v>
+      </c>
+      <c r="M1131" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="N1131" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="O1131" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="P1131" s="4">
+        <v>78</v>
+      </c>
+      <c r="Q1131" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1131" s="3">
+        <v>-0.22</v>
+      </c>
+      <c r="S1131" s="2"/>
+    </row>
+    <row r="1132" spans="12:19" ht="15.75" thickBot="1">
+      <c r="L1132" s="2" t="s">
+        <v>735</v>
+      </c>
+      <c r="M1132" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="N1132" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="O1132" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="P1132" s="4">
+        <v>100</v>
+      </c>
+      <c r="Q1132" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1132" s="3"/>
+      <c r="S1132" s="2"/>
+    </row>
+    <row r="1133" spans="12:19" ht="15.75" thickBot="1">
+      <c r="L1133" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="M1133" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1133" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="O1133" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="P1133" s="4">
+        <v>64</v>
+      </c>
+      <c r="Q1133" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1133" s="5">
+        <v>0.22</v>
+      </c>
+      <c r="S1133" s="2"/>
+    </row>
+    <row r="1134" spans="12:19" ht="15.75" thickBot="1">
+      <c r="L1134" s="2" t="s">
+        <v>738</v>
+      </c>
+      <c r="M1134" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1134" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="O1134" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="P1134" s="4">
+        <v>42</v>
+      </c>
+      <c r="Q1134" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1134" s="3"/>
+      <c r="S1134" s="2"/>
+    </row>
+    <row r="1135" spans="12:19" ht="15.75" thickBot="1">
+      <c r="L1135" s="2" t="s">
+        <v>739</v>
+      </c>
+      <c r="M1135" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N1135" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="O1135" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="P1135" s="4">
+        <v>110</v>
+      </c>
+      <c r="Q1135" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1135" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="S1135" s="2"/>
+    </row>
+    <row r="1136" spans="12:19" ht="15.75" thickBot="1">
+      <c r="L1136" s="2" t="s">
+        <v>741</v>
+      </c>
+      <c r="M1136" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N1136" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="O1136" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="P1136" s="4">
+        <v>109</v>
+      </c>
+      <c r="Q1136" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1136" s="3"/>
+      <c r="S1136" s="2"/>
+    </row>
+    <row r="1137" spans="12:19" ht="15.75" thickBot="1">
+      <c r="L1137" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="M1137" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="N1137" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="O1137" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="P1137" s="4">
+        <v>108</v>
+      </c>
+      <c r="Q1137" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1137" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="S1137" s="2"/>
+    </row>
+    <row r="1138" spans="12:19" ht="15.75" thickBot="1">
+      <c r="L1138" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="M1138" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="N1138" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="O1138" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="P1138" s="4">
+        <v>98</v>
+      </c>
+      <c r="Q1138" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1138" s="3"/>
+      <c r="S1138" s="2"/>
+    </row>
+    <row r="1139" spans="12:19" ht="15.75" thickBot="1">
+      <c r="L1139" s="2" t="s">
+        <v>745</v>
+      </c>
+      <c r="M1139" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N1139" s="2" t="s">
+        <v>746</v>
+      </c>
+      <c r="O1139" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="P1139" s="4">
+        <v>137</v>
+      </c>
+      <c r="Q1139" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1139" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="S1139" s="2"/>
+    </row>
+    <row r="1140" spans="12:19" ht="15.75" thickBot="1">
+      <c r="L1140" s="2" t="s">
+        <v>747</v>
+      </c>
+      <c r="M1140" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N1140" s="2" t="s">
+        <v>746</v>
+      </c>
+      <c r="O1140" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="P1140" s="4">
+        <v>117</v>
+      </c>
+      <c r="Q1140" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1140" s="3"/>
+      <c r="S1140" s="2"/>
+    </row>
+    <row r="1141" spans="12:19" ht="15.75" thickBot="1">
+      <c r="L1141" s="2" t="s">
+        <v>747</v>
+      </c>
+      <c r="M1141" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1141" s="2" t="s">
+        <v>748</v>
+      </c>
+      <c r="O1141" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="P1141" s="4">
+        <v>40</v>
+      </c>
+      <c r="Q1141" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1141" s="3">
+        <v>-0.11</v>
+      </c>
+      <c r="S1141" s="2"/>
+    </row>
+    <row r="1142" spans="12:19" ht="15.75" thickBot="1">
+      <c r="L1142" s="2" t="s">
+        <v>749</v>
+      </c>
+      <c r="M1142" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N1142" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="O1142" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="P1142" s="4">
+        <v>182</v>
+      </c>
+      <c r="Q1142" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1142" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="S1142" s="2"/>
+    </row>
+    <row r="1143" spans="12:19" ht="15.75" thickBot="1">
+      <c r="L1143" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="M1143" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N1143" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="O1143" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="P1143" s="4">
+        <v>122</v>
+      </c>
+      <c r="Q1143" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1143" s="3"/>
+      <c r="S1143" s="2"/>
+    </row>
+    <row r="1144" spans="12:19" ht="15.75" thickBot="1">
+      <c r="L1144" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="M1144" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N1144" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="O1144" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="P1144" s="4">
+        <v>49</v>
+      </c>
+      <c r="Q1144" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1144" s="3">
+        <v>-0.69</v>
+      </c>
+      <c r="S1144" s="2"/>
+    </row>
+    <row r="1145" spans="12:19" ht="15.75" thickBot="1">
+      <c r="L1145" s="2" t="s">
+        <v>754</v>
+      </c>
+      <c r="M1145" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1145" s="2" t="s">
+        <v>748</v>
+      </c>
+      <c r="O1145" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="P1145" s="4">
+        <v>51</v>
+      </c>
+      <c r="Q1145" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1145" s="3"/>
+      <c r="S1145" s="2"/>
+    </row>
+    <row r="1146" spans="12:19" ht="15.75" thickBot="1">
+      <c r="L1146" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="M1146" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N1146" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="O1146" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="P1146" s="4">
+        <v>118</v>
+      </c>
+      <c r="Q1146" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1146" s="3"/>
+      <c r="S1146" s="2"/>
+    </row>
+    <row r="1147" spans="12:19" ht="15.75" thickBot="1">
+      <c r="S1147" s="2"/>
+    </row>
+    <row r="1148" spans="12:19" ht="15.75" thickBot="1">
+      <c r="S1148" s="2"/>
+    </row>
+    <row r="1149" spans="12:19" ht="15.75" thickBot="1">
+      <c r="S1149" s="2"/>
+    </row>
+    <row r="1150" spans="12:19" ht="15.75" thickBot="1">
+      <c r="S1150" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20979,10 +22655,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{829BCB3E-ADB5-497C-8636-01F5B5FDB73F}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R36" sqref="R36"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21043,6 +22719,14 @@
         <v>437</v>
       </c>
       <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="21">
+        <v>45141</v>
+      </c>
+      <c r="B8">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added eurospread and spread tableau workbooks
</commit_message>
<xml_diff>
--- a/spreadex.xlsx
+++ b/spreadex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kovan\FDAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E011ED54-36AD-483D-B331-7B6A39446994}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C8AE65-E143-4DBE-852F-977B695F5B73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="802" activeTab="11" xr2:uid="{8365F371-5EDF-4C19-B0B3-71E11A5B2E12}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="802" xr2:uid="{8365F371-5EDF-4C19-B0B3-71E11A5B2E12}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4317" uniqueCount="845">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4549" uniqueCount="921">
   <si>
     <t>24/11/2022 20:55</t>
   </si>
@@ -2580,6 +2580,234 @@
   </si>
   <si>
     <t>win=15,Draw=5,Goal=10,clean sheet=5,Red card=-15</t>
+  </si>
+  <si>
+    <t>27/03/2023 21:37</t>
+  </si>
+  <si>
+    <t>Rep. Ireland v France</t>
+  </si>
+  <si>
+    <t>27/03/2023 20:12</t>
+  </si>
+  <si>
+    <t>25/03/2023 21:37</t>
+  </si>
+  <si>
+    <t>Spain v Norway</t>
+  </si>
+  <si>
+    <t>25/03/2023 19:41</t>
+  </si>
+  <si>
+    <t>25/03/2023 15:56</t>
+  </si>
+  <si>
+    <t>Scotland v Cyprus</t>
+  </si>
+  <si>
+    <t>25/03/2023 14:05</t>
+  </si>
+  <si>
+    <t>24/03/2023 21:40</t>
+  </si>
+  <si>
+    <t>France v Netherlands</t>
+  </si>
+  <si>
+    <t>24/03/2023 19:45</t>
+  </si>
+  <si>
+    <t>23/03/2023 21:44</t>
+  </si>
+  <si>
+    <t>Italy v England</t>
+  </si>
+  <si>
+    <t>23/03/2023 20:05</t>
+  </si>
+  <si>
+    <t>19/03/2023 21:58</t>
+  </si>
+  <si>
+    <t>Barcelona v Real Madrid</t>
+  </si>
+  <si>
+    <t>19/03/2023 19:29</t>
+  </si>
+  <si>
+    <t>19/03/2023 18:27</t>
+  </si>
+  <si>
+    <t>Leverkusen v Bayern Munich</t>
+  </si>
+  <si>
+    <t>19/03/2023 16:25</t>
+  </si>
+  <si>
+    <t>19/03/2023 13:27</t>
+  </si>
+  <si>
+    <t>Sampdoria v Verona</t>
+  </si>
+  <si>
+    <t>19/03/2023 11:42</t>
+  </si>
+  <si>
+    <t>18/03/2023 17:00</t>
+  </si>
+  <si>
+    <t>Southampton v Tottenham</t>
+  </si>
+  <si>
+    <t>18/03/2023 15:43</t>
+  </si>
+  <si>
+    <t>18/03/2023 12:32</t>
+  </si>
+  <si>
+    <t>Kasimpasa v Umraniyespor</t>
+  </si>
+  <si>
+    <t>18/03/2023 10:20</t>
+  </si>
+  <si>
+    <t>17/03/2023 20:57</t>
+  </si>
+  <si>
+    <t>M'Gladbach v Werder Bremen</t>
+  </si>
+  <si>
+    <t>17/03/2023 20:01</t>
+  </si>
+  <si>
+    <t>17/03/2023 19:03</t>
+  </si>
+  <si>
+    <t>Konyaspor v Galatasaray</t>
+  </si>
+  <si>
+    <t>17/03/2023 17:05</t>
+  </si>
+  <si>
+    <t>16/03/2023 21:46</t>
+  </si>
+  <si>
+    <t>Arsenal v Sporting Lisbon</t>
+  </si>
+  <si>
+    <t>16/03/2023 20:10</t>
+  </si>
+  <si>
+    <t>16/03/2023 19:47</t>
+  </si>
+  <si>
+    <t>Fenerbahce v Sevilla</t>
+  </si>
+  <si>
+    <t>16/03/2023 17:35</t>
+  </si>
+  <si>
+    <t>15/03/2023 21:55</t>
+  </si>
+  <si>
+    <t>Real Madrid v Liverpool</t>
+  </si>
+  <si>
+    <t>15/03/2023 21:28</t>
+  </si>
+  <si>
+    <t>Southampton v Brentford</t>
+  </si>
+  <si>
+    <t>15/03/2023 20:34</t>
+  </si>
+  <si>
+    <t>15/03/2023 19:37</t>
+  </si>
+  <si>
+    <t>14/03/2023 21:54</t>
+  </si>
+  <si>
+    <t>Middlesbrough v Stoke</t>
+  </si>
+  <si>
+    <t>14/03/2023 21:42</t>
+  </si>
+  <si>
+    <t>Rotherham v Preston</t>
+  </si>
+  <si>
+    <t>14/03/2023 20:50</t>
+  </si>
+  <si>
+    <t>Man City v RB Leipzig</t>
+  </si>
+  <si>
+    <t>14/03/2023 20:17</t>
+  </si>
+  <si>
+    <t>14/03/2023 20:05</t>
+  </si>
+  <si>
+    <t>14/03/2023 19:48</t>
+  </si>
+  <si>
+    <t>13/04/2023 20:19</t>
+  </si>
+  <si>
+    <t>Man Utd v Sevilla</t>
+  </si>
+  <si>
+    <t>13/04/2023 20:03</t>
+  </si>
+  <si>
+    <t>Real Madrid v Chelsea</t>
+  </si>
+  <si>
+    <t>Barcelona v Girona</t>
+  </si>
+  <si>
+    <t>Fatih Karagumruk v Fenerbahce</t>
+  </si>
+  <si>
+    <t>Istanbulspor v Fatih Karagumruk</t>
+  </si>
+  <si>
+    <t>Newcastle v Man Utd</t>
+  </si>
+  <si>
+    <t>Bologna v Udinese</t>
+  </si>
+  <si>
+    <t>Bayern Munich v Dortmund</t>
+  </si>
+  <si>
+    <t>Karlsruhe v Braunschweig</t>
+  </si>
+  <si>
+    <t>31/03/2023 21:44</t>
+  </si>
+  <si>
+    <t>Burnley v Sunderland</t>
+  </si>
+  <si>
+    <t>31/03/2023 21:24</t>
+  </si>
+  <si>
+    <t>Eintracht Frankfurt v Bochum</t>
+  </si>
+  <si>
+    <t>31/03/2023 20:10</t>
+  </si>
+  <si>
+    <t>31/03/2023 19:23</t>
+  </si>
+  <si>
+    <t>Nurnberg v Darmstadt</t>
+  </si>
+  <si>
+    <t>31/03/2023 17:58</t>
   </si>
 </sst>
 </file>
@@ -2716,7 +2944,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2827,6 +3055,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3144,13 +3375,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B2ACDE7-BC8B-432A-9773-10E95E9E94B1}">
-  <dimension ref="A1:V1251"/>
+  <dimension ref="A1:V1344"/>
   <sheetViews>
-    <sheetView zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B1222" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B1324" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I1256" sqref="I1256"/>
+      <selection pane="bottomRight" activeCell="A1343" sqref="A1343:G1344"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3163,6 +3394,7 @@
     <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" style="15" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
     <col min="10" max="10" width="15.42578125" customWidth="1"/>
     <col min="11" max="11" width="15.28515625" customWidth="1"/>
     <col min="12" max="12" width="14.140625" customWidth="1"/>
@@ -24061,8 +24293,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="1249" spans="1:7" ht="15.75" thickBot="1"/>
-    <row r="1250" spans="1:7" ht="15.75" thickBot="1">
+    <row r="1249" spans="1:17" ht="15.75" thickBot="1"/>
+    <row r="1250" spans="1:17" ht="15.75" thickBot="1">
       <c r="A1250" s="2" t="s">
         <v>761</v>
       </c>
@@ -24085,7 +24317,7 @@
         <v>-0.15</v>
       </c>
     </row>
-    <row r="1251" spans="1:7" ht="15.75" thickBot="1">
+    <row r="1251" spans="1:17" ht="15.75" thickBot="1">
       <c r="A1251" s="2" t="s">
         <v>765</v>
       </c>
@@ -24104,6 +24336,1543 @@
       <c r="F1251" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="J1251" s="1"/>
+      <c r="K1251" s="1"/>
+      <c r="L1251" s="1"/>
+      <c r="M1251" s="1"/>
+      <c r="N1251" s="1"/>
+      <c r="O1251" s="1"/>
+      <c r="P1251" s="1"/>
+      <c r="Q1251" s="1"/>
+    </row>
+    <row r="1252" spans="1:17" ht="15.75" thickBot="1">
+      <c r="Q1252" s="2"/>
+    </row>
+    <row r="1253" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1253" s="2" t="s">
+        <v>895</v>
+      </c>
+      <c r="B1253" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1253" s="2" t="s">
+        <v>896</v>
+      </c>
+      <c r="D1253" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1253" s="4">
+        <v>64</v>
+      </c>
+      <c r="F1253" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1253" s="3">
+        <v>-0.37</v>
+      </c>
+      <c r="Q1253" s="2"/>
+    </row>
+    <row r="1254" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1254" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="B1254" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1254" s="2" t="s">
+        <v>896</v>
+      </c>
+      <c r="D1254" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1254" s="4">
+        <v>101</v>
+      </c>
+      <c r="F1254" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1254" s="2"/>
+    </row>
+    <row r="1255" spans="1:17" ht="15.75" thickBot="1">
+      <c r="Q1255" s="2"/>
+    </row>
+    <row r="1256" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1256" s="2" t="s">
+        <v>897</v>
+      </c>
+      <c r="B1256" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1256" s="2" t="s">
+        <v>898</v>
+      </c>
+      <c r="D1256" s="3">
+        <v>-0.18</v>
+      </c>
+      <c r="E1256" s="4">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="F1256" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1256" s="5">
+        <v>0.35</v>
+      </c>
+      <c r="Q1256" s="2"/>
+    </row>
+    <row r="1257" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1257" s="2" t="s">
+        <v>899</v>
+      </c>
+      <c r="B1257" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1257" s="2" t="s">
+        <v>898</v>
+      </c>
+      <c r="D1257" s="5">
+        <v>0.18</v>
+      </c>
+      <c r="E1257" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="F1257" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1257" s="3"/>
+      <c r="Q1257" s="2"/>
+    </row>
+    <row r="1258" spans="1:17" ht="15.75" thickBot="1">
+      <c r="Q1258" s="2"/>
+    </row>
+    <row r="1259" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1259" s="2" t="s">
+        <v>893</v>
+      </c>
+      <c r="B1259" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1259" s="2" t="s">
+        <v>894</v>
+      </c>
+      <c r="D1259" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1259" s="4">
+        <v>100</v>
+      </c>
+      <c r="F1259" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1259" s="3">
+        <v>-0.13</v>
+      </c>
+      <c r="Q1259" s="2"/>
+    </row>
+    <row r="1260" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1260" s="2" t="s">
+        <v>900</v>
+      </c>
+      <c r="B1260" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1260" s="2" t="s">
+        <v>894</v>
+      </c>
+      <c r="D1260" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1260" s="4">
+        <v>113</v>
+      </c>
+      <c r="F1260" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1260" s="2"/>
+    </row>
+    <row r="1261" spans="1:17" ht="15.75" thickBot="1">
+      <c r="Q1261" s="2"/>
+    </row>
+    <row r="1262" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1262" s="2" t="s">
+        <v>889</v>
+      </c>
+      <c r="B1262" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1262" s="2" t="s">
+        <v>890</v>
+      </c>
+      <c r="D1262" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1262" s="4">
+        <v>36</v>
+      </c>
+      <c r="F1262" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1262" s="3">
+        <v>-0.64</v>
+      </c>
+      <c r="Q1262" s="2"/>
+    </row>
+    <row r="1263" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1263" s="2" t="s">
+        <v>892</v>
+      </c>
+      <c r="B1263" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1263" s="2" t="s">
+        <v>890</v>
+      </c>
+      <c r="D1263" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1263" s="4">
+        <v>100</v>
+      </c>
+      <c r="F1263" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1263" s="2"/>
+    </row>
+    <row r="1264" spans="1:17" ht="15.75" thickBot="1">
+      <c r="Q1264" s="2"/>
+    </row>
+    <row r="1265" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1265" s="2" t="s">
+        <v>887</v>
+      </c>
+      <c r="B1265" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1265" s="2" t="s">
+        <v>888</v>
+      </c>
+      <c r="D1265" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E1265" s="4">
+        <v>1</v>
+      </c>
+      <c r="F1265" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1265" s="3">
+        <v>-1.65</v>
+      </c>
+      <c r="Q1265" s="2"/>
+    </row>
+    <row r="1266" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1266" s="2" t="s">
+        <v>891</v>
+      </c>
+      <c r="B1266" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1266" s="2" t="s">
+        <v>888</v>
+      </c>
+      <c r="D1266" s="5">
+        <v>1</v>
+      </c>
+      <c r="E1266" s="4">
+        <v>2.65</v>
+      </c>
+      <c r="F1266" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1266" s="2"/>
+    </row>
+    <row r="1267" spans="1:17" ht="15.75" thickBot="1">
+      <c r="Q1267" s="2"/>
+    </row>
+    <row r="1268" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1268" s="2" t="s">
+        <v>884</v>
+      </c>
+      <c r="B1268" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1268" s="2" t="s">
+        <v>885</v>
+      </c>
+      <c r="D1268" s="3">
+        <v>-0.18</v>
+      </c>
+      <c r="E1268" s="4">
+        <v>1</v>
+      </c>
+      <c r="F1268" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1268" s="3">
+        <v>-0.31</v>
+      </c>
+      <c r="Q1268" s="2"/>
+    </row>
+    <row r="1269" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1269" s="2" t="s">
+        <v>886</v>
+      </c>
+      <c r="B1269" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1269" s="2" t="s">
+        <v>885</v>
+      </c>
+      <c r="D1269" s="5">
+        <v>0.18</v>
+      </c>
+      <c r="E1269" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="F1269" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1269" s="3"/>
+      <c r="Q1269" s="2"/>
+    </row>
+    <row r="1270" spans="1:17" ht="15.75" thickBot="1">
+      <c r="Q1270" s="2"/>
+    </row>
+    <row r="1271" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1271" s="2" t="s">
+        <v>881</v>
+      </c>
+      <c r="B1271" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1271" s="2" t="s">
+        <v>882</v>
+      </c>
+      <c r="D1271" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1271" s="4">
+        <v>103</v>
+      </c>
+      <c r="F1271" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1271" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="Q1271" s="2"/>
+    </row>
+    <row r="1272" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1272" s="2" t="s">
+        <v>883</v>
+      </c>
+      <c r="B1272" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1272" s="2" t="s">
+        <v>882</v>
+      </c>
+      <c r="D1272" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1272" s="4">
+        <v>100</v>
+      </c>
+      <c r="F1272" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1272" s="3"/>
+      <c r="Q1272" s="2"/>
+    </row>
+    <row r="1273" spans="1:17" ht="15.75" thickBot="1">
+      <c r="Q1273" s="2"/>
+    </row>
+    <row r="1274" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1274" s="2" t="s">
+        <v>878</v>
+      </c>
+      <c r="B1274" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1274" s="2" t="s">
+        <v>879</v>
+      </c>
+      <c r="D1274" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1274" s="4">
+        <v>100</v>
+      </c>
+      <c r="F1274" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1274" s="3">
+        <v>-0.12</v>
+      </c>
+      <c r="Q1274" s="2"/>
+    </row>
+    <row r="1275" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1275" s="2" t="s">
+        <v>880</v>
+      </c>
+      <c r="B1275" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1275" s="2" t="s">
+        <v>879</v>
+      </c>
+      <c r="D1275" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1275" s="4">
+        <v>112</v>
+      </c>
+      <c r="F1275" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1275" s="3"/>
+      <c r="Q1275" s="2"/>
+    </row>
+    <row r="1276" spans="1:17" ht="15.75" thickBot="1">
+      <c r="Q1276" s="2"/>
+    </row>
+    <row r="1277" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1277" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="B1277" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1277" s="2" t="s">
+        <v>876</v>
+      </c>
+      <c r="D1277" s="3">
+        <v>-0.18</v>
+      </c>
+      <c r="E1277" s="4">
+        <v>3</v>
+      </c>
+      <c r="F1277" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1277" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="Q1277" s="2"/>
+    </row>
+    <row r="1278" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1278" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="B1278" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1278" s="2" t="s">
+        <v>876</v>
+      </c>
+      <c r="D1278" s="5">
+        <v>0.18</v>
+      </c>
+      <c r="E1278" s="4">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="F1278" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1278" s="3"/>
+      <c r="Q1278" s="2"/>
+    </row>
+    <row r="1279" spans="1:17" ht="15.75" thickBot="1">
+      <c r="Q1279" s="2"/>
+    </row>
+    <row r="1280" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1280" s="2" t="s">
+        <v>872</v>
+      </c>
+      <c r="B1280" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1280" s="2" t="s">
+        <v>873</v>
+      </c>
+      <c r="D1280" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1280" s="4">
+        <v>92</v>
+      </c>
+      <c r="F1280" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1280" s="3">
+        <v>-0.15</v>
+      </c>
+      <c r="Q1280" s="2"/>
+    </row>
+    <row r="1281" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1281" s="2" t="s">
+        <v>874</v>
+      </c>
+      <c r="B1281" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1281" s="2" t="s">
+        <v>873</v>
+      </c>
+      <c r="D1281" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1281" s="4">
+        <v>107</v>
+      </c>
+      <c r="F1281" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1281" s="3"/>
+      <c r="Q1281" s="2"/>
+    </row>
+    <row r="1282" spans="1:17" ht="15.75" thickBot="1">
+      <c r="P1282" s="3"/>
+      <c r="Q1282" s="2"/>
+    </row>
+    <row r="1283" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1283" s="2" t="s">
+        <v>869</v>
+      </c>
+      <c r="B1283" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1283" s="2" t="s">
+        <v>870</v>
+      </c>
+      <c r="D1283" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1283" s="4">
+        <v>20</v>
+      </c>
+      <c r="F1283" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1283" s="3">
+        <v>-0.08</v>
+      </c>
+      <c r="P1283" s="3"/>
+      <c r="Q1283" s="2"/>
+    </row>
+    <row r="1284" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1284" s="2" t="s">
+        <v>871</v>
+      </c>
+      <c r="B1284" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1284" s="2" t="s">
+        <v>870</v>
+      </c>
+      <c r="D1284" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1284" s="4">
+        <v>28</v>
+      </c>
+      <c r="F1284" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1284" s="3"/>
+      <c r="Q1284" s="2"/>
+    </row>
+    <row r="1285" spans="1:17" ht="15.75" thickBot="1">
+      <c r="Q1285" s="2"/>
+    </row>
+    <row r="1286" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1286" s="2" t="s">
+        <v>866</v>
+      </c>
+      <c r="B1286" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1286" s="2" t="s">
+        <v>867</v>
+      </c>
+      <c r="D1286" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1286" s="4">
+        <v>50</v>
+      </c>
+      <c r="F1286" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1286" s="3">
+        <v>-0.04</v>
+      </c>
+      <c r="Q1286" s="2"/>
+    </row>
+    <row r="1287" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1287" s="2" t="s">
+        <v>868</v>
+      </c>
+      <c r="B1287" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1287" s="2" t="s">
+        <v>867</v>
+      </c>
+      <c r="D1287" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1287" s="4">
+        <v>54</v>
+      </c>
+      <c r="F1287" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1287" s="3"/>
+      <c r="Q1287" s="2"/>
+    </row>
+    <row r="1288" spans="1:17" ht="15.75" thickBot="1">
+      <c r="P1288" s="3"/>
+      <c r="Q1288" s="2"/>
+    </row>
+    <row r="1289" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1289" s="2" t="s">
+        <v>863</v>
+      </c>
+      <c r="B1289" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1289" s="2" t="s">
+        <v>864</v>
+      </c>
+      <c r="D1289" s="3">
+        <v>-0.18</v>
+      </c>
+      <c r="E1289" s="4">
+        <v>3</v>
+      </c>
+      <c r="F1289" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1289" s="3">
+        <v>-0.08</v>
+      </c>
+      <c r="P1289" s="3"/>
+      <c r="Q1289" s="2"/>
+    </row>
+    <row r="1290" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1290" s="2" t="s">
+        <v>865</v>
+      </c>
+      <c r="B1290" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1290" s="2" t="s">
+        <v>864</v>
+      </c>
+      <c r="D1290" s="5">
+        <v>0.18</v>
+      </c>
+      <c r="E1290" s="4">
+        <v>3.45</v>
+      </c>
+      <c r="F1290" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1290" s="3"/>
+    </row>
+    <row r="1291" spans="1:17" ht="15.75" thickBot="1"/>
+    <row r="1292" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1292" s="2" t="s">
+        <v>860</v>
+      </c>
+      <c r="B1292" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1292" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="D1292" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1292" s="4">
+        <v>107</v>
+      </c>
+      <c r="F1292" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1292" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J1292" s="1"/>
+      <c r="K1292" s="1"/>
+      <c r="L1292" s="1"/>
+      <c r="M1292" s="1"/>
+      <c r="N1292" s="1"/>
+      <c r="O1292" s="1"/>
+      <c r="P1292" s="1"/>
+      <c r="Q1292" s="1"/>
+    </row>
+    <row r="1293" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1293" s="2" t="s">
+        <v>862</v>
+      </c>
+      <c r="B1293" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1293" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="D1293" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1293" s="4">
+        <v>100</v>
+      </c>
+      <c r="F1293" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1293" s="3"/>
+      <c r="Q1293" s="2"/>
+    </row>
+    <row r="1294" spans="1:17" ht="15.75" thickBot="1">
+      <c r="Q1294" s="2"/>
+    </row>
+    <row r="1295" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1295" s="2" t="s">
+        <v>857</v>
+      </c>
+      <c r="B1295" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1295" s="2" t="s">
+        <v>858</v>
+      </c>
+      <c r="D1295" s="3">
+        <v>-0.18</v>
+      </c>
+      <c r="E1295" s="4">
+        <v>3</v>
+      </c>
+      <c r="F1295" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1295" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q1295" s="2"/>
+    </row>
+    <row r="1296" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1296" s="2" t="s">
+        <v>859</v>
+      </c>
+      <c r="B1296" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1296" s="2" t="s">
+        <v>858</v>
+      </c>
+      <c r="D1296" s="5">
+        <v>0.18</v>
+      </c>
+      <c r="E1296" s="4">
+        <v>3</v>
+      </c>
+      <c r="F1296" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1296" s="3"/>
+      <c r="Q1296" s="2"/>
+    </row>
+    <row r="1297" spans="1:17" ht="15.75" thickBot="1">
+      <c r="Q1297" s="2"/>
+    </row>
+    <row r="1298" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1298" s="2" t="s">
+        <v>845</v>
+      </c>
+      <c r="B1298" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1298" s="2" t="s">
+        <v>846</v>
+      </c>
+      <c r="D1298" s="3">
+        <v>-0.18</v>
+      </c>
+      <c r="E1298" s="4">
+        <v>1</v>
+      </c>
+      <c r="F1298" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1298" s="3">
+        <v>-0.18</v>
+      </c>
+      <c r="Q1298" s="2"/>
+    </row>
+    <row r="1299" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1299" s="2" t="s">
+        <v>847</v>
+      </c>
+      <c r="B1299" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1299" s="2" t="s">
+        <v>846</v>
+      </c>
+      <c r="D1299" s="5">
+        <v>0.18</v>
+      </c>
+      <c r="E1299" s="4">
+        <v>2</v>
+      </c>
+      <c r="F1299" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1299" s="3"/>
+      <c r="Q1299" s="2"/>
+    </row>
+    <row r="1300" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1300" s="2"/>
+      <c r="B1300" s="2"/>
+      <c r="C1300" s="2"/>
+      <c r="D1300" s="5"/>
+      <c r="E1300" s="4"/>
+      <c r="F1300" s="2"/>
+      <c r="G1300" s="3"/>
+      <c r="H1300" s="40"/>
+      <c r="Q1300" s="2"/>
+    </row>
+    <row r="1301" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1301" s="2" t="s">
+        <v>848</v>
+      </c>
+      <c r="B1301" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1301" s="2" t="s">
+        <v>849</v>
+      </c>
+      <c r="D1301" s="3">
+        <v>-0.18</v>
+      </c>
+      <c r="E1301" s="4">
+        <v>3</v>
+      </c>
+      <c r="F1301" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1301" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="Q1301" s="2"/>
+    </row>
+    <row r="1302" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1302" s="2" t="s">
+        <v>850</v>
+      </c>
+      <c r="B1302" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1302" s="2" t="s">
+        <v>849</v>
+      </c>
+      <c r="D1302" s="5">
+        <v>0.18</v>
+      </c>
+      <c r="E1302" s="4">
+        <v>2.9</v>
+      </c>
+      <c r="F1302" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1302" s="3"/>
+      <c r="Q1302" s="2"/>
+    </row>
+    <row r="1303" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1303" s="2"/>
+      <c r="B1303" s="2"/>
+      <c r="C1303" s="2"/>
+      <c r="D1303" s="5"/>
+      <c r="E1303" s="4"/>
+      <c r="F1303" s="2"/>
+      <c r="G1303" s="3"/>
+      <c r="H1303" s="40"/>
+      <c r="Q1303" s="2"/>
+    </row>
+    <row r="1304" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1304" s="2" t="s">
+        <v>851</v>
+      </c>
+      <c r="B1304" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1304" s="2" t="s">
+        <v>852</v>
+      </c>
+      <c r="D1304" s="3">
+        <v>-0.18</v>
+      </c>
+      <c r="E1304" s="4">
+        <v>3</v>
+      </c>
+      <c r="F1304" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1304" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q1304" s="2"/>
+    </row>
+    <row r="1305" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1305" s="2" t="s">
+        <v>853</v>
+      </c>
+      <c r="B1305" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1305" s="2" t="s">
+        <v>852</v>
+      </c>
+      <c r="D1305" s="5">
+        <v>0.18</v>
+      </c>
+      <c r="E1305" s="4">
+        <v>3</v>
+      </c>
+      <c r="F1305" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1305" s="3"/>
+      <c r="Q1305" s="2"/>
+    </row>
+    <row r="1306" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1306" s="2"/>
+      <c r="B1306" s="2"/>
+      <c r="C1306" s="2"/>
+      <c r="D1306" s="5"/>
+      <c r="E1306" s="4"/>
+      <c r="F1306" s="2"/>
+      <c r="G1306" s="3"/>
+      <c r="H1306" s="40"/>
+      <c r="J1306" s="11"/>
+      <c r="K1306" s="2"/>
+      <c r="L1306" s="2"/>
+      <c r="M1306" s="3"/>
+      <c r="N1306" s="4"/>
+      <c r="O1306" s="2"/>
+      <c r="P1306" s="3"/>
+      <c r="Q1306" s="2"/>
+    </row>
+    <row r="1307" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1307" s="2" t="s">
+        <v>854</v>
+      </c>
+      <c r="B1307" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1307" s="2" t="s">
+        <v>855</v>
+      </c>
+      <c r="D1307" s="3">
+        <v>-0.18</v>
+      </c>
+      <c r="E1307" s="4">
+        <v>4</v>
+      </c>
+      <c r="F1307" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1307" s="5">
+        <v>0.22</v>
+      </c>
+      <c r="P1307" s="3"/>
+      <c r="Q1307" s="2"/>
+    </row>
+    <row r="1308" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1308" s="2" t="s">
+        <v>856</v>
+      </c>
+      <c r="B1308" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1308" s="2" t="s">
+        <v>855</v>
+      </c>
+      <c r="D1308" s="5">
+        <v>0.18</v>
+      </c>
+      <c r="E1308" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="F1308" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1308" s="3"/>
+      <c r="Q1308" s="2"/>
+    </row>
+    <row r="1309" spans="1:17" ht="15.75" thickBot="1">
+      <c r="Q1309" s="2"/>
+    </row>
+    <row r="1310" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1310" s="2" t="s">
+        <v>918</v>
+      </c>
+      <c r="B1310" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1310" s="2" t="s">
+        <v>919</v>
+      </c>
+      <c r="D1310" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="E1310" s="4">
+        <v>1</v>
+      </c>
+      <c r="F1310" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1310" s="3">
+        <v>-0.18</v>
+      </c>
+      <c r="Q1310" s="2"/>
+    </row>
+    <row r="1311" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1311" s="2" t="s">
+        <v>920</v>
+      </c>
+      <c r="B1311" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1311" s="2" t="s">
+        <v>919</v>
+      </c>
+      <c r="D1311" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="E1311" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="F1311" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1311" s="3"/>
+      <c r="Q1311" s="2"/>
+    </row>
+    <row r="1312" spans="1:17" ht="15.75" thickBot="1">
+      <c r="Q1312" s="2"/>
+    </row>
+    <row r="1313" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1313" s="2" t="s">
+        <v>915</v>
+      </c>
+      <c r="B1313" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1313" s="2" t="s">
+        <v>916</v>
+      </c>
+      <c r="D1313" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="E1313" s="4">
+        <v>2</v>
+      </c>
+      <c r="F1313" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1313" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="Q1313" s="2"/>
+    </row>
+    <row r="1314" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1314" s="2" t="s">
+        <v>918</v>
+      </c>
+      <c r="B1314" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1314" s="2" t="s">
+        <v>916</v>
+      </c>
+      <c r="D1314" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="E1314" s="4">
+        <v>3</v>
+      </c>
+      <c r="F1314" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1314" s="2"/>
+    </row>
+    <row r="1315" spans="1:17" ht="15.75" thickBot="1">
+      <c r="Q1315" s="2"/>
+    </row>
+    <row r="1316" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1316" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="B1316" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1316" s="2" t="s">
+        <v>914</v>
+      </c>
+      <c r="D1316" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1316" s="4">
+        <v>103</v>
+      </c>
+      <c r="F1316" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1316" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="P1316" s="3"/>
+      <c r="Q1316" s="2"/>
+    </row>
+    <row r="1317" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1317" s="2" t="s">
+        <v>917</v>
+      </c>
+      <c r="B1317" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1317" s="2" t="s">
+        <v>914</v>
+      </c>
+      <c r="D1317" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1317" s="4">
+        <v>100</v>
+      </c>
+      <c r="F1317" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1317" s="3"/>
+      <c r="Q1317" s="2"/>
+    </row>
+    <row r="1318" spans="1:17" ht="15.75" thickBot="1">
+      <c r="Q1318" s="2"/>
+    </row>
+    <row r="1319" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1319" s="11">
+        <v>44930.579861111109</v>
+      </c>
+      <c r="B1319" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1319" s="2" t="s">
+        <v>912</v>
+      </c>
+      <c r="D1319" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="E1319" s="4">
+        <v>2</v>
+      </c>
+      <c r="F1319" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1319" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="Q1319" s="2"/>
+    </row>
+    <row r="1320" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1320" s="11">
+        <v>44930.502083333333</v>
+      </c>
+      <c r="B1320" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1320" s="2" t="s">
+        <v>912</v>
+      </c>
+      <c r="D1320" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="E1320" s="4">
+        <v>3</v>
+      </c>
+      <c r="F1320" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1320" s="3"/>
+    </row>
+    <row r="1321" spans="1:17" ht="15.75" thickBot="1"/>
+    <row r="1322" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1322" s="11">
+        <v>44930.743055555555</v>
+      </c>
+      <c r="B1322" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1322" s="2" t="s">
+        <v>911</v>
+      </c>
+      <c r="D1322" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1322" s="4">
+        <v>125</v>
+      </c>
+      <c r="F1322" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1322" s="5">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="1323" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1323" s="11">
+        <v>44930.722222222219</v>
+      </c>
+      <c r="B1323" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1323" s="2" t="s">
+        <v>911</v>
+      </c>
+      <c r="D1323" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1323" s="4">
+        <v>107</v>
+      </c>
+      <c r="F1323" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1323" s="3"/>
+    </row>
+    <row r="1324" spans="1:17" ht="15.75" thickBot="1"/>
+    <row r="1325" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1325" s="11">
+        <v>44961.497916666667</v>
+      </c>
+      <c r="B1325" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1325" s="2" t="s">
+        <v>910</v>
+      </c>
+      <c r="D1325" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1325" s="4">
+        <v>152</v>
+      </c>
+      <c r="F1325" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1325" s="5">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="1326" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1326" s="11">
+        <v>44961.481944444444</v>
+      </c>
+      <c r="B1326" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1326" s="2" t="s">
+        <v>910</v>
+      </c>
+      <c r="D1326" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1326" s="4">
+        <v>103</v>
+      </c>
+      <c r="F1326" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1326" s="3"/>
+    </row>
+    <row r="1327" spans="1:17" ht="15.75" thickBot="1"/>
+    <row r="1328" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1328" s="11">
+        <v>44961.76666666667</v>
+      </c>
+      <c r="B1328" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1328" s="2" t="s">
+        <v>909</v>
+      </c>
+      <c r="D1328" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1328" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1328" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1328" s="3">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="1329" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A1329" s="11">
+        <v>44961.700694444444</v>
+      </c>
+      <c r="B1329" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1329" s="2" t="s">
+        <v>909</v>
+      </c>
+      <c r="D1329" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1329" s="4">
+        <v>50</v>
+      </c>
+      <c r="F1329" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1330" spans="1:15" ht="15.75" thickBot="1"/>
+    <row r="1331" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A1331" s="11">
+        <v>44989.852777777778</v>
+      </c>
+      <c r="B1331" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1331" s="2" t="s">
+        <v>908</v>
+      </c>
+      <c r="D1331" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="E1331" s="4">
+        <v>1</v>
+      </c>
+      <c r="F1331" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1331" s="3">
+        <v>-0.38</v>
+      </c>
+    </row>
+    <row r="1332" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A1332" s="11">
+        <v>44989.768750000003</v>
+      </c>
+      <c r="B1332" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1332" s="2" t="s">
+        <v>908</v>
+      </c>
+      <c r="D1332" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="E1332" s="4">
+        <v>3</v>
+      </c>
+      <c r="F1332" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1332" s="3"/>
+    </row>
+    <row r="1333" spans="1:15" ht="15.75" thickBot="1"/>
+    <row r="1334" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A1334" s="11">
+        <v>45203.824305555558</v>
+      </c>
+      <c r="B1334" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1334" s="2" t="s">
+        <v>907</v>
+      </c>
+      <c r="D1334" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="E1334" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="F1334" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1334" s="5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="1335" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A1335" s="11">
+        <v>45203.784722222219</v>
+      </c>
+      <c r="B1335" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1335" s="2" t="s">
+        <v>907</v>
+      </c>
+      <c r="D1335" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="E1335" s="4">
+        <v>3</v>
+      </c>
+      <c r="F1335" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1336" spans="1:15" ht="15.75" thickBot="1"/>
+    <row r="1337" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A1337" s="11">
+        <v>45203.848611111112</v>
+      </c>
+      <c r="B1337" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1337" s="2" t="s">
+        <v>906</v>
+      </c>
+      <c r="D1337" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1337" s="4">
+        <v>134</v>
+      </c>
+      <c r="F1337" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1337" s="5">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="1338" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A1338" s="11">
+        <v>45203.838194444441</v>
+      </c>
+      <c r="B1338" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1338" s="2" t="s">
+        <v>906</v>
+      </c>
+      <c r="D1338" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1338" s="4">
+        <v>94</v>
+      </c>
+      <c r="F1338" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1338" s="3"/>
+    </row>
+    <row r="1339" spans="1:15" ht="15.75" thickBot="1"/>
+    <row r="1340" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A1340" s="11">
+        <v>45264.898611111108</v>
+      </c>
+      <c r="B1340" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1340" s="2" t="s">
+        <v>905</v>
+      </c>
+      <c r="D1340" s="3">
+        <v>-0.18</v>
+      </c>
+      <c r="E1340" s="4">
+        <v>2.65</v>
+      </c>
+      <c r="F1340" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1340" s="5">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="1341" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A1341" s="11">
+        <v>45264.822916666664</v>
+      </c>
+      <c r="B1341" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1341" s="2" t="s">
+        <v>905</v>
+      </c>
+      <c r="D1341" s="5">
+        <v>0.18</v>
+      </c>
+      <c r="E1341" s="4">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="F1341" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1341" s="3"/>
+      <c r="I1341" s="11"/>
+      <c r="J1341" s="2"/>
+      <c r="K1341" s="2"/>
+      <c r="L1341" s="3"/>
+      <c r="M1341" s="4"/>
+      <c r="N1341" s="2"/>
+      <c r="O1341" s="5"/>
+    </row>
+    <row r="1342" spans="1:15" ht="15.75" thickBot="1">
+      <c r="O1342" s="3"/>
+    </row>
+    <row r="1343" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A1343" s="2" t="s">
+        <v>902</v>
+      </c>
+      <c r="B1343" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1343" s="2" t="s">
+        <v>903</v>
+      </c>
+      <c r="D1343" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1343" s="4">
+        <v>146</v>
+      </c>
+      <c r="F1343" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1343" s="5">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="1344" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A1344" s="2" t="s">
+        <v>904</v>
+      </c>
+      <c r="B1344" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1344" s="2" t="s">
+        <v>903</v>
+      </c>
+      <c r="D1344" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1344" s="4">
+        <v>108</v>
+      </c>
+      <c r="F1344" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1344" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24113,10 +25882,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{829BCB3E-ADB5-497C-8636-01F5B5FDB73F}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B8"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24185,6 +25954,14 @@
         <v>45141</v>
       </c>
       <c r="B8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="21">
+        <v>45203</v>
+      </c>
+      <c r="B9">
         <v>5</v>
       </c>
     </row>
@@ -24231,7 +26008,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4A182E3-C93B-4DB5-AEB9-9967F8A10B1A}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+    <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
       <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
@@ -24581,17 +26358,17 @@
       <c r="C32">
         <v>1.5</v>
       </c>
-      <c r="D32" s="40" t="s">
+      <c r="D32" s="41" t="s">
         <v>841</v>
       </c>
-      <c r="E32" s="40"/>
-      <c r="F32" s="40"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="40"/>
-      <c r="I32" s="40"/>
-      <c r="J32" s="40"/>
-      <c r="K32" s="40"/>
-      <c r="L32" s="40"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="41"/>
+      <c r="J32" s="41"/>
+      <c r="K32" s="41"/>
+      <c r="L32" s="41"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
@@ -24600,14 +26377,14 @@
       <c r="B33" t="s">
         <v>843</v>
       </c>
-      <c r="C33" s="40" t="s">
+      <c r="C33" s="41" t="s">
         <v>844</v>
       </c>
-      <c r="D33" s="40"/>
-      <c r="E33" s="40"/>
-      <c r="F33" s="40"/>
-      <c r="G33" s="40"/>
-      <c r="H33" s="40"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="41"/>
+      <c r="H33" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
updated leagues and odds
</commit_message>
<xml_diff>
--- a/spreadex.xlsx
+++ b/spreadex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kovan\FDAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E14E8B7-4BA8-453B-94DD-452C98565461}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD8E5E6-6886-40E6-811A-F264F0960016}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="802" xr2:uid="{8365F371-5EDF-4C19-B0B3-71E11A5B2E12}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4741" uniqueCount="990">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4861" uniqueCount="1024">
   <si>
     <t>24/11/2022 20:55</t>
   </si>
@@ -3015,6 +3015,108 @@
   </si>
   <si>
     <t>14/04/2023 18:36</t>
+  </si>
+  <si>
+    <t>Nottingham Forest v Southampton</t>
+  </si>
+  <si>
+    <t>West Ham v Man Utd</t>
+  </si>
+  <si>
+    <t>Dortmund v Wolfsburg</t>
+  </si>
+  <si>
+    <t>Atalanta v Juventus</t>
+  </si>
+  <si>
+    <t>M'Gladbach v Bochum</t>
+  </si>
+  <si>
+    <t>Karlsruhe v Hannover</t>
+  </si>
+  <si>
+    <t>Blackburn v Luton</t>
+  </si>
+  <si>
+    <t>Rotherham v Middlesbrough</t>
+  </si>
+  <si>
+    <t>30/04/2023 16:11</t>
+  </si>
+  <si>
+    <t>Bayern Munich v Hertha BSC</t>
+  </si>
+  <si>
+    <t>30/04/2023 15:01</t>
+  </si>
+  <si>
+    <t>30/04/2023 13:34</t>
+  </si>
+  <si>
+    <t>Monaco v Montpellier</t>
+  </si>
+  <si>
+    <t>30/04/2023 13:27</t>
+  </si>
+  <si>
+    <t>Inter Milan v Lazio</t>
+  </si>
+  <si>
+    <t>30/04/2023 12:11</t>
+  </si>
+  <si>
+    <t>30/04/2023 11:32</t>
+  </si>
+  <si>
+    <t>29/04/2023 16:27</t>
+  </si>
+  <si>
+    <t>Eintracht Frankfurt v Augsburg</t>
+  </si>
+  <si>
+    <t>29/04/2023 14:41</t>
+  </si>
+  <si>
+    <t>28/04/2023 19:42</t>
+  </si>
+  <si>
+    <t>28/04/2023 19:36</t>
+  </si>
+  <si>
+    <t>28/04/2023 19:19</t>
+  </si>
+  <si>
+    <t>Lecce v Udinese</t>
+  </si>
+  <si>
+    <t>28/04/2023 17:41</t>
+  </si>
+  <si>
+    <t>27/04/2023 21:45</t>
+  </si>
+  <si>
+    <t>Tottenham v Man Utd</t>
+  </si>
+  <si>
+    <t>27/04/2023 20:35</t>
+  </si>
+  <si>
+    <t>27/04/2023 20:28</t>
+  </si>
+  <si>
+    <t>Valencia v Valladolid</t>
+  </si>
+  <si>
+    <t>27/04/2023 18:30</t>
+  </si>
+  <si>
+    <t>26/04/2023 21:58</t>
+  </si>
+  <si>
+    <t>Man City v Arsenal</t>
+  </si>
+  <si>
+    <t>26/04/2023 19:47</t>
   </si>
 </sst>
 </file>
@@ -3151,7 +3253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3268,6 +3370,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3582,13 +3685,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B2ACDE7-BC8B-432A-9773-10E95E9E94B1}">
-  <dimension ref="A1:V1393"/>
+  <dimension ref="A1:V1467"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B1354" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B1435" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G1351" sqref="G1351"/>
+      <selection pane="bottomRight" activeCell="K1464" sqref="K1464"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -26113,27 +26216,6 @@
       <c r="G1346" s="3">
         <v>-0.64</v>
       </c>
-      <c r="I1346" s="2" t="s">
-        <v>921</v>
-      </c>
-      <c r="J1346" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1346" s="2" t="s">
-        <v>922</v>
-      </c>
-      <c r="L1346" s="3">
-        <v>-0.01</v>
-      </c>
-      <c r="M1346" s="4">
-        <v>47</v>
-      </c>
-      <c r="N1346" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O1346" s="3">
-        <v>-0.06</v>
-      </c>
       <c r="P1346" s="2"/>
     </row>
     <row r="1347" spans="1:16" ht="15.75" thickBot="1">
@@ -26155,1045 +26237,1953 @@
       <c r="F1347" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1347" s="2" t="s">
-        <v>923</v>
-      </c>
-      <c r="J1347" s="2" t="s">
+      <c r="P1347" s="2"/>
+    </row>
+    <row r="1348" spans="1:16" ht="15.75" thickBot="1">
+      <c r="P1348" s="2"/>
+    </row>
+    <row r="1349" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1349" s="2" t="s">
+        <v>984</v>
+      </c>
+      <c r="B1349" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1349" s="2" t="s">
+        <v>985</v>
+      </c>
+      <c r="D1349" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1349" s="4">
+        <v>25</v>
+      </c>
+      <c r="F1349" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1349" s="3">
+        <v>-0.88</v>
+      </c>
+      <c r="P1349" s="2"/>
+    </row>
+    <row r="1350" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1350" s="2" t="s">
+        <v>988</v>
+      </c>
+      <c r="B1350" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1350" s="2" t="s">
+        <v>985</v>
+      </c>
+      <c r="D1350" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1350" s="4">
+        <v>113</v>
+      </c>
+      <c r="F1350" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1350" s="3"/>
+      <c r="P1350" s="2"/>
+    </row>
+    <row r="1351" spans="1:16" ht="15.75" thickBot="1">
+      <c r="P1351" s="2"/>
+    </row>
+    <row r="1352" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1352" s="2" t="s">
+        <v>981</v>
+      </c>
+      <c r="B1352" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1352" s="2" t="s">
+        <v>982</v>
+      </c>
+      <c r="D1352" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1352" s="4">
+        <v>142</v>
+      </c>
+      <c r="F1352" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1352" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="P1352" s="2"/>
+    </row>
+    <row r="1353" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1353" s="2" t="s">
+        <v>983</v>
+      </c>
+      <c r="B1353" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1353" s="2" t="s">
+        <v>982</v>
+      </c>
+      <c r="D1353" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1353" s="4">
+        <v>123</v>
+      </c>
+      <c r="F1353" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1353" s="3"/>
+      <c r="P1353" s="2"/>
+    </row>
+    <row r="1354" spans="1:16" ht="15.75" thickBot="1">
+      <c r="P1354" s="2"/>
+    </row>
+    <row r="1355" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1355" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="B1355" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1355" s="2" t="s">
+        <v>977</v>
+      </c>
+      <c r="D1355" s="3">
+        <v>-0.2</v>
+      </c>
+      <c r="E1355" s="4">
+        <v>4</v>
+      </c>
+      <c r="F1355" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1355" s="5">
+        <v>0.26</v>
+      </c>
+      <c r="P1355" s="2"/>
+    </row>
+    <row r="1356" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1356" s="2" t="s">
+        <v>979</v>
+      </c>
+      <c r="B1356" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1356" s="2" t="s">
+        <v>977</v>
+      </c>
+      <c r="D1356" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="E1356" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="F1356" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1356" s="3"/>
+      <c r="P1356" s="2"/>
+    </row>
+    <row r="1357" spans="1:16" ht="15.75" thickBot="1">
+      <c r="P1357" s="2"/>
+    </row>
+    <row r="1358" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1358" s="2" t="s">
+        <v>976</v>
+      </c>
+      <c r="B1358" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1358" s="2" t="s">
+        <v>977</v>
+      </c>
+      <c r="D1358" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1358" s="4">
+        <v>116</v>
+      </c>
+      <c r="F1358" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1358" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="P1358" s="2"/>
+    </row>
+    <row r="1359" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1359" s="2" t="s">
+        <v>980</v>
+      </c>
+      <c r="B1359" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1359" s="2" t="s">
+        <v>977</v>
+      </c>
+      <c r="D1359" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1359" s="4">
+        <v>106</v>
+      </c>
+      <c r="F1359" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1359" s="2"/>
+    </row>
+    <row r="1360" spans="1:16" ht="15.75" thickBot="1">
+      <c r="P1360" s="2"/>
+    </row>
+    <row r="1361" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1361" s="2" t="s">
+        <v>973</v>
+      </c>
+      <c r="B1361" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1361" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="D1361" s="3">
+        <v>-0.18</v>
+      </c>
+      <c r="E1361" s="4">
+        <v>5</v>
+      </c>
+      <c r="F1361" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1361" s="5">
+        <v>0.35</v>
+      </c>
+      <c r="P1361" s="2"/>
+    </row>
+    <row r="1362" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1362" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="B1362" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1362" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="D1362" s="5">
+        <v>0.18</v>
+      </c>
+      <c r="E1362" s="4">
+        <v>3.05</v>
+      </c>
+      <c r="F1362" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1362" s="3"/>
+      <c r="P1362" s="2"/>
+    </row>
+    <row r="1363" spans="1:16" ht="15.75" thickBot="1">
+      <c r="P1363" s="2"/>
+    </row>
+    <row r="1364" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1364" s="2" t="s">
+        <v>970</v>
+      </c>
+      <c r="B1364" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K1347" s="2" t="s">
-        <v>922</v>
-      </c>
-      <c r="L1347" s="5">
+      <c r="C1364" s="2" t="s">
+        <v>971</v>
+      </c>
+      <c r="D1364" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1364" s="4">
+        <v>75</v>
+      </c>
+      <c r="F1364" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1364" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="P1364" s="2"/>
+    </row>
+    <row r="1365" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1365" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="B1365" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1365" s="2" t="s">
+        <v>971</v>
+      </c>
+      <c r="D1365" s="5">
         <v>0.01</v>
       </c>
-      <c r="M1347" s="4">
-        <v>53</v>
-      </c>
-      <c r="N1347" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1347" s="3"/>
-      <c r="P1347" s="2"/>
-    </row>
-    <row r="1348" spans="1:16" ht="15.75" thickBot="1">
-      <c r="I1348" s="2" t="s">
-        <v>924</v>
-      </c>
-      <c r="J1348" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1348" s="2" t="s">
-        <v>925</v>
-      </c>
-      <c r="L1348" s="3">
+      <c r="E1365" s="4">
+        <v>68</v>
+      </c>
+      <c r="F1365" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1365" s="3"/>
+      <c r="P1365" s="2"/>
+    </row>
+    <row r="1366" spans="1:16" ht="15.75" thickBot="1">
+      <c r="P1366" s="2"/>
+    </row>
+    <row r="1367" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1367" s="2" t="s">
+        <v>967</v>
+      </c>
+      <c r="B1367" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1367" s="2" t="s">
+        <v>968</v>
+      </c>
+      <c r="D1367" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="E1367" s="4">
+        <v>2</v>
+      </c>
+      <c r="F1367" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1367" s="3">
+        <v>-0.15</v>
+      </c>
+      <c r="P1367" s="2"/>
+    </row>
+    <row r="1368" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1368" s="2" t="s">
+        <v>969</v>
+      </c>
+      <c r="B1368" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1368" s="2" t="s">
+        <v>968</v>
+      </c>
+      <c r="D1368" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="E1368" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="F1368" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1368" s="3"/>
+      <c r="P1368" s="2"/>
+    </row>
+    <row r="1369" spans="1:16" ht="15.75" thickBot="1">
+      <c r="P1369" s="2"/>
+    </row>
+    <row r="1370" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1370" s="2" t="s">
+        <v>962</v>
+      </c>
+      <c r="B1370" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1370" s="2" t="s">
+        <v>963</v>
+      </c>
+      <c r="D1370" s="3">
         <v>-0.01</v>
       </c>
-      <c r="M1348" s="4">
-        <v>44</v>
-      </c>
-      <c r="N1348" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O1348" s="3">
-        <v>-0.16</v>
-      </c>
-      <c r="P1348" s="2"/>
-    </row>
-    <row r="1349" spans="1:16" ht="15.75" thickBot="1">
-      <c r="I1349" s="2" t="s">
-        <v>926</v>
-      </c>
-      <c r="J1349" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1349" s="2" t="s">
-        <v>925</v>
-      </c>
-      <c r="L1349" s="5">
+      <c r="E1370" s="4">
+        <v>49</v>
+      </c>
+      <c r="F1370" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1370" s="3">
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="P1370" s="2"/>
+    </row>
+    <row r="1371" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1371" s="2" t="s">
+        <v>966</v>
+      </c>
+      <c r="B1371" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1371" s="2" t="s">
+        <v>963</v>
+      </c>
+      <c r="D1371" s="5">
         <v>0.01</v>
       </c>
-      <c r="M1349" s="4">
-        <v>60</v>
-      </c>
-      <c r="N1349" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1349" s="3"/>
-      <c r="P1349" s="2"/>
-    </row>
-    <row r="1350" spans="1:16" ht="15.75" thickBot="1">
-      <c r="I1350" s="2" t="s">
-        <v>927</v>
-      </c>
-      <c r="J1350" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="K1350" s="2" t="s">
-        <v>928</v>
-      </c>
-      <c r="L1350" s="3">
-        <v>-0.01</v>
-      </c>
-      <c r="M1350" s="4">
-        <v>49</v>
-      </c>
-      <c r="N1350" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1350" s="3">
-        <v>-0.49</v>
-      </c>
-      <c r="P1350" s="2"/>
-    </row>
-    <row r="1351" spans="1:16" ht="15.75" thickBot="1">
-      <c r="I1351" s="2" t="s">
-        <v>929</v>
-      </c>
-      <c r="J1351" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="K1351" s="2" t="s">
-        <v>928</v>
-      </c>
-      <c r="L1351" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="M1351" s="4">
-        <v>98</v>
-      </c>
-      <c r="N1351" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1351" s="3"/>
-      <c r="P1351" s="2"/>
-    </row>
-    <row r="1352" spans="1:16" ht="15.75" thickBot="1">
-      <c r="I1352" s="2" t="s">
-        <v>930</v>
-      </c>
-      <c r="J1352" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1352" s="2" t="s">
-        <v>931</v>
-      </c>
-      <c r="L1352" s="3">
-        <v>-0.5</v>
-      </c>
-      <c r="M1352" s="4">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="N1352" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O1352" s="5">
-        <v>0.45</v>
-      </c>
-      <c r="P1352" s="2"/>
-    </row>
-    <row r="1353" spans="1:16" ht="15.75" thickBot="1">
-      <c r="I1353" s="2" t="s">
-        <v>932</v>
-      </c>
-      <c r="J1353" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1353" s="2" t="s">
-        <v>933</v>
-      </c>
-      <c r="L1353" s="3">
-        <v>-0.19</v>
-      </c>
-      <c r="M1353" s="4">
-        <v>3.8</v>
-      </c>
-      <c r="N1353" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O1353" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="P1353" s="2"/>
-    </row>
-    <row r="1354" spans="1:16" ht="15.75" thickBot="1">
-      <c r="I1354" s="2" t="s">
-        <v>934</v>
-      </c>
-      <c r="J1354" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1354" s="2" t="s">
-        <v>931</v>
-      </c>
-      <c r="L1354" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="M1354" s="4">
-        <v>3.45</v>
-      </c>
-      <c r="N1354" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1354" s="3"/>
-      <c r="P1354" s="2"/>
-    </row>
-    <row r="1355" spans="1:16" ht="15.75" thickBot="1">
-      <c r="I1355" s="2" t="s">
-        <v>935</v>
-      </c>
-      <c r="J1355" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1355" s="2" t="s">
-        <v>933</v>
-      </c>
-      <c r="L1355" s="5">
-        <v>0.19</v>
-      </c>
-      <c r="M1355" s="4">
-        <v>2.75</v>
-      </c>
-      <c r="N1355" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1355" s="3"/>
-      <c r="P1355" s="2"/>
-    </row>
-    <row r="1356" spans="1:16" ht="15.75" thickBot="1">
-      <c r="I1356" s="2" t="s">
-        <v>936</v>
-      </c>
-      <c r="J1356" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1356" s="2" t="s">
-        <v>937</v>
-      </c>
-      <c r="L1356" s="3">
-        <v>-0.2</v>
-      </c>
-      <c r="M1356" s="4">
-        <v>2.4500000000000002</v>
-      </c>
-      <c r="N1356" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O1356" s="5">
-        <v>0.11</v>
-      </c>
-      <c r="P1356" s="2"/>
-    </row>
-    <row r="1357" spans="1:16" ht="15.75" thickBot="1">
-      <c r="I1357" s="2" t="s">
-        <v>938</v>
-      </c>
-      <c r="J1357" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1357" s="2" t="s">
-        <v>937</v>
-      </c>
-      <c r="L1357" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="M1357" s="4">
-        <v>1.9</v>
-      </c>
-      <c r="N1357" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1357" s="3"/>
-      <c r="P1357" s="2"/>
-    </row>
-    <row r="1358" spans="1:16" ht="15.75" thickBot="1">
-      <c r="I1358" s="2" t="s">
-        <v>939</v>
-      </c>
-      <c r="J1358" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="K1358" s="2" t="s">
-        <v>940</v>
-      </c>
-      <c r="L1358" s="3">
-        <v>-0.01</v>
-      </c>
-      <c r="M1358" s="4">
-        <v>123</v>
-      </c>
-      <c r="N1358" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O1358" s="5">
-        <v>0.24</v>
-      </c>
-      <c r="P1358" s="2"/>
-    </row>
-    <row r="1359" spans="1:16" ht="15.75" thickBot="1">
-      <c r="I1359" s="2" t="s">
-        <v>941</v>
-      </c>
-      <c r="J1359" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="K1359" s="2" t="s">
-        <v>940</v>
-      </c>
-      <c r="L1359" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="M1359" s="4">
-        <v>99</v>
-      </c>
-      <c r="N1359" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1359" s="3"/>
-      <c r="P1359" s="2"/>
-    </row>
-    <row r="1360" spans="1:16" ht="15.75" thickBot="1">
-      <c r="I1360" s="2" t="s">
-        <v>942</v>
-      </c>
-      <c r="J1360" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1360" s="2" t="s">
-        <v>943</v>
-      </c>
-      <c r="L1360" s="3">
-        <v>-0.19</v>
-      </c>
-      <c r="M1360" s="4">
-        <v>3</v>
-      </c>
-      <c r="N1360" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1360" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="P1360" s="2"/>
-    </row>
-    <row r="1361" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1361" s="2" t="s">
-        <v>944</v>
-      </c>
-      <c r="J1361" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1361" s="2" t="s">
-        <v>943</v>
-      </c>
-      <c r="L1361" s="5">
-        <v>0.19</v>
-      </c>
-      <c r="M1361" s="4">
-        <v>2.95</v>
-      </c>
-      <c r="N1361" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1361" s="3"/>
-      <c r="P1361" s="2"/>
-    </row>
-    <row r="1362" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1362" s="2" t="s">
-        <v>945</v>
-      </c>
-      <c r="J1362" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1362" s="2" t="s">
-        <v>946</v>
-      </c>
-      <c r="L1362" s="3">
-        <v>-0.01</v>
-      </c>
-      <c r="M1362" s="4">
-        <v>20</v>
-      </c>
-      <c r="N1362" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1362" s="3">
-        <v>-0.28000000000000003</v>
-      </c>
-      <c r="P1362" s="2"/>
-    </row>
-    <row r="1363" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1363" s="2" t="s">
-        <v>947</v>
-      </c>
-      <c r="J1363" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1363" s="2" t="s">
-        <v>948</v>
-      </c>
-      <c r="L1363" s="3">
-        <v>-0.19</v>
-      </c>
-      <c r="M1363" s="4">
-        <v>2</v>
-      </c>
-      <c r="N1363" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1363" s="5">
-        <v>0.03</v>
-      </c>
-      <c r="P1363" s="2"/>
-    </row>
-    <row r="1364" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1364" s="2" t="s">
-        <v>949</v>
-      </c>
-      <c r="J1364" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1364" s="2" t="s">
-        <v>946</v>
-      </c>
-      <c r="L1364" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="M1364" s="4">
-        <v>48</v>
-      </c>
-      <c r="N1364" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1364" s="3"/>
-      <c r="P1364" s="2"/>
-    </row>
-    <row r="1365" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1365" s="2" t="s">
-        <v>950</v>
-      </c>
-      <c r="J1365" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1365" s="2" t="s">
-        <v>948</v>
-      </c>
-      <c r="L1365" s="5">
-        <v>0.19</v>
-      </c>
-      <c r="M1365" s="4">
-        <v>1.85</v>
-      </c>
-      <c r="N1365" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1365" s="3"/>
-      <c r="P1365" s="2"/>
-    </row>
-    <row r="1366" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1366" s="2" t="s">
-        <v>951</v>
-      </c>
-      <c r="J1366" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="K1366" s="2" t="s">
-        <v>952</v>
-      </c>
-      <c r="L1366" s="3">
-        <v>-0.01</v>
-      </c>
-      <c r="M1366" s="4">
-        <v>81</v>
-      </c>
-      <c r="N1366" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1366" s="3">
-        <v>-0.4</v>
-      </c>
-      <c r="P1366" s="2"/>
-    </row>
-    <row r="1367" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1367" s="2" t="s">
-        <v>953</v>
-      </c>
-      <c r="J1367" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="K1367" s="2" t="s">
-        <v>952</v>
-      </c>
-      <c r="L1367" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="M1367" s="4">
-        <v>121</v>
-      </c>
-      <c r="N1367" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1367" s="3"/>
-      <c r="P1367" s="2"/>
-    </row>
-    <row r="1368" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1368" s="2" t="s">
-        <v>954</v>
-      </c>
-      <c r="J1368" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="K1368" s="2" t="s">
-        <v>955</v>
-      </c>
-      <c r="L1368" s="3">
-        <v>-0.01</v>
-      </c>
-      <c r="M1368" s="4">
-        <v>36</v>
-      </c>
-      <c r="N1368" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1368" s="3">
-        <v>-0.77</v>
-      </c>
-      <c r="P1368" s="2"/>
-    </row>
-    <row r="1369" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1369" s="2" t="s">
-        <v>956</v>
-      </c>
-      <c r="J1369" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="K1369" s="2" t="s">
-        <v>955</v>
-      </c>
-      <c r="L1369" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="M1369" s="4">
-        <v>113</v>
-      </c>
-      <c r="N1369" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1369" s="3"/>
-      <c r="P1369" s="2"/>
-    </row>
-    <row r="1370" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1370" s="2" t="s">
-        <v>957</v>
-      </c>
-      <c r="J1370" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1370" s="2" t="s">
-        <v>958</v>
-      </c>
-      <c r="L1370" s="3">
-        <v>-0.01</v>
-      </c>
-      <c r="M1370" s="4">
-        <v>40</v>
-      </c>
-      <c r="N1370" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1370" s="3">
-        <v>-0.15</v>
-      </c>
-      <c r="P1370" s="2"/>
-    </row>
-    <row r="1371" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1371" s="2" t="s">
-        <v>959</v>
-      </c>
-      <c r="J1371" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="K1371" s="2" t="s">
-        <v>958</v>
-      </c>
-      <c r="L1371" s="3">
-        <v>-0.01</v>
-      </c>
-      <c r="M1371" s="4">
-        <v>126</v>
-      </c>
-      <c r="N1371" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O1371" s="5">
-        <v>0.15</v>
-      </c>
+      <c r="E1371" s="4">
+        <v>104</v>
+      </c>
+      <c r="F1371" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1371" s="3"/>
       <c r="P1371" s="2"/>
     </row>
-    <row r="1372" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1372" s="2" t="s">
-        <v>960</v>
-      </c>
-      <c r="J1372" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1372" s="2" t="s">
-        <v>958</v>
-      </c>
-      <c r="L1372" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="M1372" s="4">
-        <v>55</v>
-      </c>
-      <c r="N1372" s="2" t="s">
-        <v>5</v>
-      </c>
+    <row r="1372" spans="1:16" ht="15.75" thickBot="1">
       <c r="O1372" s="3"/>
       <c r="P1372" s="2"/>
     </row>
-    <row r="1373" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1373" s="2" t="s">
-        <v>961</v>
-      </c>
-      <c r="J1373" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="K1373" s="2" t="s">
-        <v>958</v>
-      </c>
-      <c r="L1373" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="M1373" s="4">
-        <v>111</v>
-      </c>
-      <c r="N1373" s="2" t="s">
-        <v>5</v>
+    <row r="1373" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1373" s="2" t="s">
+        <v>964</v>
+      </c>
+      <c r="B1373" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1373" s="2" t="s">
+        <v>963</v>
+      </c>
+      <c r="D1373" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1373" s="4">
+        <v>90</v>
+      </c>
+      <c r="F1373" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1373" s="5">
+        <v>0.41</v>
       </c>
       <c r="O1373" s="3"/>
       <c r="P1373" s="2"/>
     </row>
-    <row r="1374" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1374" s="2" t="s">
-        <v>962</v>
-      </c>
-      <c r="J1374" s="2" t="s">
+    <row r="1374" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1374" s="2" t="s">
+        <v>965</v>
+      </c>
+      <c r="B1374" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1374" s="2" t="s">
+        <v>963</v>
+      </c>
+      <c r="D1374" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1374" s="4">
+        <v>49</v>
+      </c>
+      <c r="F1374" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1374" s="3"/>
+      <c r="P1374" s="2"/>
+    </row>
+    <row r="1375" spans="1:16" ht="15.75" thickBot="1">
+      <c r="P1375" s="2"/>
+    </row>
+    <row r="1376" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1376" s="2" t="s">
+        <v>959</v>
+      </c>
+      <c r="B1376" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="K1374" s="2" t="s">
-        <v>963</v>
-      </c>
-      <c r="L1374" s="3">
+      <c r="C1376" s="2" t="s">
+        <v>958</v>
+      </c>
+      <c r="D1376" s="3">
         <v>-0.01</v>
       </c>
-      <c r="M1374" s="4">
+      <c r="E1376" s="4">
+        <v>126</v>
+      </c>
+      <c r="F1376" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1376" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="P1376" s="2"/>
+    </row>
+    <row r="1377" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1377" s="2" t="s">
+        <v>961</v>
+      </c>
+      <c r="B1377" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1377" s="2" t="s">
+        <v>958</v>
+      </c>
+      <c r="D1377" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1377" s="4">
+        <v>111</v>
+      </c>
+      <c r="F1377" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1377" s="2"/>
+    </row>
+    <row r="1378" spans="1:16" ht="15.75" thickBot="1">
+      <c r="P1378" s="2"/>
+    </row>
+    <row r="1379" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1379" s="2" t="s">
+        <v>957</v>
+      </c>
+      <c r="B1379" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1379" s="2" t="s">
+        <v>958</v>
+      </c>
+      <c r="D1379" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1379" s="4">
+        <v>40</v>
+      </c>
+      <c r="F1379" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1379" s="3">
+        <v>-0.15</v>
+      </c>
+      <c r="P1379" s="2"/>
+    </row>
+    <row r="1380" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1380" s="2" t="s">
+        <v>960</v>
+      </c>
+      <c r="B1380" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1380" s="2" t="s">
+        <v>958</v>
+      </c>
+      <c r="D1380" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1380" s="4">
+        <v>55</v>
+      </c>
+      <c r="F1380" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1380" s="2"/>
+    </row>
+    <row r="1381" spans="1:16" ht="15.75" thickBot="1">
+      <c r="P1381" s="2"/>
+    </row>
+    <row r="1382" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1382" s="2" t="s">
+        <v>954</v>
+      </c>
+      <c r="B1382" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1382" s="2" t="s">
+        <v>955</v>
+      </c>
+      <c r="D1382" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1382" s="4">
+        <v>36</v>
+      </c>
+      <c r="F1382" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1382" s="3">
+        <v>-0.77</v>
+      </c>
+      <c r="P1382" s="2"/>
+    </row>
+    <row r="1383" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1383" s="2" t="s">
+        <v>956</v>
+      </c>
+      <c r="B1383" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1383" s="2" t="s">
+        <v>955</v>
+      </c>
+      <c r="D1383" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1383" s="4">
+        <v>113</v>
+      </c>
+      <c r="F1383" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1383" s="3"/>
+      <c r="P1383" s="2"/>
+    </row>
+    <row r="1384" spans="1:16" ht="15.75" thickBot="1">
+      <c r="P1384" s="2"/>
+    </row>
+    <row r="1385" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1385" s="2" t="s">
+        <v>951</v>
+      </c>
+      <c r="B1385" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1385" s="2" t="s">
+        <v>952</v>
+      </c>
+      <c r="D1385" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1385" s="4">
+        <v>81</v>
+      </c>
+      <c r="F1385" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1385" s="3">
+        <v>-0.4</v>
+      </c>
+      <c r="P1385" s="2"/>
+    </row>
+    <row r="1386" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1386" s="2" t="s">
+        <v>953</v>
+      </c>
+      <c r="B1386" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1386" s="2" t="s">
+        <v>952</v>
+      </c>
+      <c r="D1386" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1386" s="4">
+        <v>121</v>
+      </c>
+      <c r="F1386" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1386" s="3"/>
+      <c r="P1386" s="2"/>
+    </row>
+    <row r="1387" spans="1:16" ht="15.75" thickBot="1">
+      <c r="P1387" s="2"/>
+    </row>
+    <row r="1388" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1388" s="2" t="s">
+        <v>947</v>
+      </c>
+      <c r="B1388" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1388" s="2" t="s">
+        <v>948</v>
+      </c>
+      <c r="D1388" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="E1388" s="4">
+        <v>2</v>
+      </c>
+      <c r="F1388" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1388" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="P1388" s="2"/>
+    </row>
+    <row r="1389" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1389" s="2" t="s">
+        <v>950</v>
+      </c>
+      <c r="B1389" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1389" s="2" t="s">
+        <v>948</v>
+      </c>
+      <c r="D1389" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="E1389" s="4">
+        <v>1.85</v>
+      </c>
+      <c r="F1389" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1389" s="2"/>
+    </row>
+    <row r="1390" spans="1:16" ht="15.75" thickBot="1">
+      <c r="P1390" s="2"/>
+    </row>
+    <row r="1391" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1391" s="2" t="s">
+        <v>945</v>
+      </c>
+      <c r="B1391" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1391" s="2" t="s">
+        <v>946</v>
+      </c>
+      <c r="D1391" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1391" s="4">
+        <v>20</v>
+      </c>
+      <c r="F1391" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1391" s="3">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="P1391" s="2"/>
+    </row>
+    <row r="1392" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1392" s="2" t="s">
+        <v>949</v>
+      </c>
+      <c r="B1392" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1392" s="2" t="s">
+        <v>946</v>
+      </c>
+      <c r="D1392" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1392" s="4">
+        <v>48</v>
+      </c>
+      <c r="F1392" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1392" s="2"/>
+    </row>
+    <row r="1393" spans="1:16" ht="15.75" thickBot="1">
+      <c r="P1393" s="2"/>
+    </row>
+    <row r="1394" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1394" s="2" t="s">
+        <v>942</v>
+      </c>
+      <c r="B1394" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1394" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="D1394" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="E1394" s="4">
+        <v>3</v>
+      </c>
+      <c r="F1394" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1394" s="5">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1395" s="2" t="s">
+        <v>944</v>
+      </c>
+      <c r="B1395" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1395" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="D1395" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="E1395" s="4">
+        <v>2.95</v>
+      </c>
+      <c r="F1395" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1395" s="3"/>
+      <c r="O1395" s="3"/>
+    </row>
+    <row r="1396" spans="1:16" ht="15.75" thickBot="1">
+      <c r="O1396" s="3"/>
+    </row>
+    <row r="1397" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1397" s="2" t="s">
+        <v>939</v>
+      </c>
+      <c r="B1397" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1397" s="2" t="s">
+        <v>940</v>
+      </c>
+      <c r="D1397" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1397" s="4">
+        <v>123</v>
+      </c>
+      <c r="F1397" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1397" s="5">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1398" s="2" t="s">
+        <v>941</v>
+      </c>
+      <c r="B1398" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1398" s="2" t="s">
+        <v>940</v>
+      </c>
+      <c r="D1398" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1398" s="4">
+        <v>99</v>
+      </c>
+      <c r="F1398" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1398" s="3"/>
+    </row>
+    <row r="1399" spans="1:16" ht="15.75" thickBot="1"/>
+    <row r="1400" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1400" s="2" t="s">
+        <v>936</v>
+      </c>
+      <c r="B1400" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1400" s="2" t="s">
+        <v>937</v>
+      </c>
+      <c r="D1400" s="3">
+        <v>-0.2</v>
+      </c>
+      <c r="E1400" s="4">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="F1400" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1400" s="5">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1401" s="2" t="s">
+        <v>938</v>
+      </c>
+      <c r="B1401" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1401" s="2" t="s">
+        <v>937</v>
+      </c>
+      <c r="D1401" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="E1401" s="4">
+        <v>1.9</v>
+      </c>
+      <c r="F1401" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1401" s="3"/>
+    </row>
+    <row r="1402" spans="1:16" ht="15.75" thickBot="1"/>
+    <row r="1403" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1403" s="2" t="s">
+        <v>932</v>
+      </c>
+      <c r="B1403" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1403" s="2" t="s">
+        <v>933</v>
+      </c>
+      <c r="D1403" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="E1403" s="4">
+        <v>3.8</v>
+      </c>
+      <c r="F1403" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1403" s="5">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1404" s="2" t="s">
+        <v>935</v>
+      </c>
+      <c r="B1404" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1404" s="2" t="s">
+        <v>933</v>
+      </c>
+      <c r="D1404" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="E1404" s="4">
+        <v>2.75</v>
+      </c>
+      <c r="F1404" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:16" ht="15.75" thickBot="1">
+      <c r="O1405" s="3"/>
+    </row>
+    <row r="1406" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1406" s="2" t="s">
+        <v>930</v>
+      </c>
+      <c r="B1406" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1406" s="2" t="s">
+        <v>931</v>
+      </c>
+      <c r="D1406" s="3">
+        <v>-0.5</v>
+      </c>
+      <c r="E1406" s="4">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="F1406" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1406" s="5">
+        <v>0.45</v>
+      </c>
+      <c r="O1406" s="3"/>
+    </row>
+    <row r="1407" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1407" s="2" t="s">
+        <v>934</v>
+      </c>
+      <c r="B1407" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1407" s="2" t="s">
+        <v>931</v>
+      </c>
+      <c r="D1407" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E1407" s="4">
+        <v>3.45</v>
+      </c>
+      <c r="F1407" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:16" ht="15.75" thickBot="1"/>
+    <row r="1409" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1409" s="2" t="s">
+        <v>927</v>
+      </c>
+      <c r="B1409" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1409" s="2" t="s">
+        <v>928</v>
+      </c>
+      <c r="D1409" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1409" s="4">
         <v>49</v>
       </c>
-      <c r="N1374" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1374" s="3">
-        <v>-0.55000000000000004</v>
-      </c>
-      <c r="P1374" s="2"/>
-    </row>
-    <row r="1375" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1375" s="2" t="s">
-        <v>964</v>
-      </c>
-      <c r="J1375" s="2" t="s">
+      <c r="F1409" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1409" s="3">
+        <v>-0.49</v>
+      </c>
+    </row>
+    <row r="1410" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1410" s="2" t="s">
+        <v>929</v>
+      </c>
+      <c r="B1410" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1410" s="2" t="s">
+        <v>928</v>
+      </c>
+      <c r="D1410" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1410" s="4">
+        <v>98</v>
+      </c>
+      <c r="F1410" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1410" s="3"/>
+    </row>
+    <row r="1411" spans="1:16" ht="15.75" thickBot="1"/>
+    <row r="1412" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1412" s="2" t="s">
+        <v>924</v>
+      </c>
+      <c r="B1412" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K1375" s="2" t="s">
-        <v>963</v>
-      </c>
-      <c r="L1375" s="3">
+      <c r="C1412" s="2" t="s">
+        <v>925</v>
+      </c>
+      <c r="D1412" s="3">
         <v>-0.01</v>
       </c>
-      <c r="M1375" s="4">
-        <v>90</v>
-      </c>
-      <c r="N1375" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1375" s="5">
-        <v>0.41</v>
-      </c>
-      <c r="P1375" s="2"/>
-    </row>
-    <row r="1376" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1376" s="2" t="s">
-        <v>965</v>
-      </c>
-      <c r="J1376" s="2" t="s">
+      <c r="E1412" s="4">
+        <v>44</v>
+      </c>
+      <c r="F1412" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1412" s="3">
+        <v>-0.16</v>
+      </c>
+    </row>
+    <row r="1413" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1413" s="2" t="s">
+        <v>926</v>
+      </c>
+      <c r="B1413" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K1376" s="2" t="s">
-        <v>963</v>
-      </c>
-      <c r="L1376" s="5">
+      <c r="C1413" s="2" t="s">
+        <v>925</v>
+      </c>
+      <c r="D1413" s="5">
         <v>0.01</v>
       </c>
-      <c r="M1376" s="4">
-        <v>49</v>
-      </c>
-      <c r="N1376" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1376" s="3"/>
-      <c r="P1376" s="2"/>
-    </row>
-    <row r="1377" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1377" s="2" t="s">
-        <v>966</v>
-      </c>
-      <c r="J1377" s="2" t="s">
+      <c r="E1413" s="4">
+        <v>60</v>
+      </c>
+      <c r="F1413" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1413" s="3"/>
+    </row>
+    <row r="1414" spans="1:16" ht="15.75" thickBot="1"/>
+    <row r="1415" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1415" s="2" t="s">
+        <v>921</v>
+      </c>
+      <c r="B1415" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1415" s="2" t="s">
+        <v>922</v>
+      </c>
+      <c r="D1415" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1415" s="4">
+        <v>47</v>
+      </c>
+      <c r="F1415" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1415" s="3">
+        <v>-0.06</v>
+      </c>
+    </row>
+    <row r="1416" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1416" s="2" t="s">
+        <v>923</v>
+      </c>
+      <c r="B1416" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1416" s="2" t="s">
+        <v>922</v>
+      </c>
+      <c r="D1416" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1416" s="4">
+        <v>53</v>
+      </c>
+      <c r="F1416" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1416" s="3"/>
+    </row>
+    <row r="1417" spans="1:16" ht="15.75" thickBot="1">
+      <c r="I1417" s="42"/>
+      <c r="J1417" s="42"/>
+      <c r="K1417" s="42"/>
+      <c r="L1417" s="42"/>
+      <c r="M1417" s="42"/>
+      <c r="N1417" s="42"/>
+      <c r="O1417" s="42"/>
+      <c r="P1417" s="42"/>
+    </row>
+    <row r="1418" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1418" s="2" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B1418" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1418" s="2" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D1418" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="E1418" s="4">
+        <v>5</v>
+      </c>
+      <c r="F1418" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1418" s="5">
+        <v>0.38</v>
+      </c>
+      <c r="P1418" s="2"/>
+    </row>
+    <row r="1419" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1419" s="2" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B1419" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1419" s="2" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D1419" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="E1419" s="4">
+        <v>3</v>
+      </c>
+      <c r="F1419" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1419" s="3"/>
+      <c r="P1419" s="2"/>
+    </row>
+    <row r="1420" spans="1:16" ht="15.75" thickBot="1">
+      <c r="P1420" s="2"/>
+    </row>
+    <row r="1421" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1421" s="2" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B1421" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="K1377" s="2" t="s">
-        <v>963</v>
-      </c>
-      <c r="L1377" s="5">
+      <c r="C1421" s="2" t="s">
+        <v>1019</v>
+      </c>
+      <c r="D1421" s="3">
+        <v>-0.02</v>
+      </c>
+      <c r="E1421" s="4">
+        <v>64</v>
+      </c>
+      <c r="F1421" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1421" s="3">
+        <v>-1.18</v>
+      </c>
+      <c r="P1421" s="2"/>
+    </row>
+    <row r="1422" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1422" s="2" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B1422" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1422" s="2" t="s">
+        <v>1019</v>
+      </c>
+      <c r="D1422" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="E1422" s="4">
+        <v>123</v>
+      </c>
+      <c r="F1422" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1422" s="3"/>
+      <c r="P1422" s="2"/>
+    </row>
+    <row r="1423" spans="1:16" ht="15.75" thickBot="1">
+      <c r="P1423" s="2"/>
+    </row>
+    <row r="1424" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1424" s="2" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B1424" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1424" s="2" t="s">
+        <v>1016</v>
+      </c>
+      <c r="D1424" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1424" s="4">
+        <v>45</v>
+      </c>
+      <c r="F1424" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1424" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="P1424" s="2"/>
+    </row>
+    <row r="1425" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1425" s="2" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B1425" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1425" s="2" t="s">
+        <v>1016</v>
+      </c>
+      <c r="D1425" s="5">
         <v>0.01</v>
       </c>
-      <c r="M1377" s="4">
-        <v>104</v>
-      </c>
-      <c r="N1377" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1377" s="3"/>
-      <c r="P1377" s="2"/>
-    </row>
-    <row r="1378" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1378" s="2" t="s">
-        <v>967</v>
-      </c>
-      <c r="J1378" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1378" s="2" t="s">
-        <v>968</v>
-      </c>
-      <c r="L1378" s="3">
+      <c r="E1425" s="4">
+        <v>43</v>
+      </c>
+      <c r="F1425" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1425" s="3"/>
+      <c r="P1425" s="2"/>
+    </row>
+    <row r="1426" spans="1:16" ht="15.75" thickBot="1">
+      <c r="P1426" s="2"/>
+    </row>
+    <row r="1427" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1427" s="2" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B1427" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1427" s="2" t="s">
+        <v>1013</v>
+      </c>
+      <c r="D1427" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1427" s="4">
+        <v>75</v>
+      </c>
+      <c r="F1427" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1427" s="3">
         <v>-0.19</v>
       </c>
-      <c r="M1378" s="4">
-        <v>2</v>
-      </c>
-      <c r="N1378" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1378" s="3">
-        <v>-0.15</v>
-      </c>
-      <c r="P1378" s="2"/>
-    </row>
-    <row r="1379" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1379" s="2" t="s">
-        <v>969</v>
-      </c>
-      <c r="J1379" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1379" s="2" t="s">
-        <v>968</v>
-      </c>
-      <c r="L1379" s="5">
+      <c r="P1427" s="2"/>
+    </row>
+    <row r="1428" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1428" s="2" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B1428" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1428" s="2" t="s">
+        <v>1013</v>
+      </c>
+      <c r="D1428" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1428" s="4">
+        <v>94</v>
+      </c>
+      <c r="F1428" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1428" s="3"/>
+      <c r="P1428" s="2"/>
+    </row>
+    <row r="1429" spans="1:16" ht="15.75" thickBot="1">
+      <c r="P1429" s="2"/>
+    </row>
+    <row r="1430" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1430" s="2" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B1430" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1430" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="D1430" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1430" s="4">
+        <v>128</v>
+      </c>
+      <c r="F1430" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1430" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="P1430" s="2"/>
+    </row>
+    <row r="1431" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1431" s="2" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B1431" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1431" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="D1431" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1431" s="4">
+        <v>105</v>
+      </c>
+      <c r="F1431" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1431" s="3"/>
+      <c r="P1431" s="2"/>
+    </row>
+    <row r="1432" spans="1:16" ht="15.75" thickBot="1">
+      <c r="P1432" s="2"/>
+    </row>
+    <row r="1433" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1433" s="2" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B1433" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1433" s="2" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D1433" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1433" s="4">
+        <v>144</v>
+      </c>
+      <c r="F1433" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1433" s="5">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="P1433" s="2"/>
+    </row>
+    <row r="1434" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1434" s="2" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B1434" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1434" s="2" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D1434" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1434" s="4">
+        <v>86</v>
+      </c>
+      <c r="F1434" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1434" s="3"/>
+      <c r="P1434" s="2"/>
+    </row>
+    <row r="1435" spans="1:16" ht="15.75" thickBot="1">
+      <c r="P1435" s="2"/>
+    </row>
+    <row r="1436" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1436" s="2" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B1436" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1436" s="2" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D1436" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1436" s="4">
+        <v>25</v>
+      </c>
+      <c r="F1436" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1436" s="3">
+        <v>-0.76</v>
+      </c>
+      <c r="P1436" s="2"/>
+    </row>
+    <row r="1437" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1437" s="2" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B1437" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1437" s="2" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D1437" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1437" s="4">
+        <v>101</v>
+      </c>
+      <c r="F1437" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1437" s="2"/>
+    </row>
+    <row r="1438" spans="1:16" ht="15.75" thickBot="1">
+      <c r="O1438" s="3"/>
+      <c r="P1438" s="2"/>
+    </row>
+    <row r="1439" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1439" s="2" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B1439" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="C1439" s="2" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D1439" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1439" s="4">
+        <v>59</v>
+      </c>
+      <c r="F1439" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1439" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="O1439" s="3"/>
+      <c r="P1439" s="2"/>
+    </row>
+    <row r="1440" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1440" s="2" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B1440" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="C1440" s="2" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D1440" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1440" s="4">
+        <v>57</v>
+      </c>
+      <c r="F1440" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1440" s="2"/>
+    </row>
+    <row r="1441" spans="1:16" ht="15.75" thickBot="1">
+      <c r="P1441" s="2"/>
+    </row>
+    <row r="1442" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1442" s="2" t="s">
+        <v>998</v>
+      </c>
+      <c r="B1442" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1442" s="2" t="s">
+        <v>999</v>
+      </c>
+      <c r="D1442" s="3">
+        <v>-0.2</v>
+      </c>
+      <c r="E1442" s="4">
+        <v>2.6</v>
+      </c>
+      <c r="F1442" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1442" s="3">
+        <v>-0.13</v>
+      </c>
+      <c r="P1442" s="2"/>
+    </row>
+    <row r="1443" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1443" s="2" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B1443" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1443" s="2" t="s">
+        <v>999</v>
+      </c>
+      <c r="D1443" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="E1443" s="4">
+        <v>3.25</v>
+      </c>
+      <c r="F1443" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1443" s="3"/>
+      <c r="P1443" s="2"/>
+    </row>
+    <row r="1444" spans="1:16" ht="15.75" thickBot="1">
+      <c r="P1444" s="2"/>
+    </row>
+    <row r="1445" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1445" s="11">
+        <v>44931.624305555553</v>
+      </c>
+      <c r="B1445" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1445" s="2" t="s">
+        <v>997</v>
+      </c>
+      <c r="D1445" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="E1445" s="4">
+        <v>1</v>
+      </c>
+      <c r="F1445" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1445" s="3">
+        <v>-0.26</v>
+      </c>
+      <c r="P1445" s="2"/>
+    </row>
+    <row r="1446" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1446" s="11">
+        <v>44931.558333333334</v>
+      </c>
+      <c r="B1446" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1446" s="2" t="s">
+        <v>997</v>
+      </c>
+      <c r="D1446" s="5">
         <v>0.19</v>
       </c>
-      <c r="M1379" s="4">
-        <v>2.8</v>
-      </c>
-      <c r="N1379" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1379" s="3"/>
-      <c r="P1379" s="2"/>
-    </row>
-    <row r="1380" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1380" s="2" t="s">
-        <v>970</v>
-      </c>
-      <c r="J1380" s="2" t="s">
+      <c r="E1446" s="4">
+        <v>2.35</v>
+      </c>
+      <c r="F1446" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1446" s="3"/>
+      <c r="P1446" s="2"/>
+    </row>
+    <row r="1447" spans="1:16" ht="15.75" thickBot="1">
+      <c r="P1447" s="2"/>
+    </row>
+    <row r="1448" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1448" s="11">
+        <v>44931.752083333333</v>
+      </c>
+      <c r="B1448" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1448" s="2" t="s">
+        <v>996</v>
+      </c>
+      <c r="D1448" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1448" s="4">
+        <v>139</v>
+      </c>
+      <c r="F1448" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1448" s="5">
+        <v>0.26</v>
+      </c>
+      <c r="I1448" s="2"/>
+      <c r="J1448" s="2"/>
+      <c r="K1448" s="2"/>
+      <c r="L1448" s="3"/>
+      <c r="M1448" s="4"/>
+      <c r="N1448" s="2"/>
+      <c r="O1448" s="3"/>
+      <c r="P1448" s="2"/>
+    </row>
+    <row r="1449" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1449" s="11">
+        <v>44931.730555555558</v>
+      </c>
+      <c r="B1449" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1449" s="2" t="s">
+        <v>996</v>
+      </c>
+      <c r="D1449" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1449" s="4">
+        <v>113</v>
+      </c>
+      <c r="F1449" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1449" s="3"/>
+      <c r="I1449" s="2"/>
+      <c r="J1449" s="2"/>
+      <c r="K1449" s="2"/>
+      <c r="L1449" s="5"/>
+      <c r="M1449" s="4"/>
+      <c r="N1449" s="2"/>
+      <c r="O1449" s="3"/>
+      <c r="P1449" s="2"/>
+    </row>
+    <row r="1450" spans="1:16" ht="15.75" thickBot="1">
+      <c r="P1450" s="2"/>
+    </row>
+    <row r="1451" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1451" s="11">
+        <v>45082.577777777777</v>
+      </c>
+      <c r="B1451" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1451" s="2" t="s">
+        <v>995</v>
+      </c>
+      <c r="D1451" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1451" s="4">
+        <v>107</v>
+      </c>
+      <c r="F1451" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1451" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="P1451" s="2"/>
+    </row>
+    <row r="1452" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1452" s="11">
+        <v>45082.504166666666</v>
+      </c>
+      <c r="B1452" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1452" s="2" t="s">
+        <v>995</v>
+      </c>
+      <c r="D1452" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1452" s="4">
+        <v>108</v>
+      </c>
+      <c r="F1452" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1452" s="3"/>
+    </row>
+    <row r="1453" spans="1:16" ht="15.75" thickBot="1"/>
+    <row r="1454" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1454" s="11">
+        <v>45082.628472222219</v>
+      </c>
+      <c r="B1454" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1454" s="2" t="s">
+        <v>994</v>
+      </c>
+      <c r="D1454" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1454" s="4">
+        <v>107</v>
+      </c>
+      <c r="F1454" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1454" s="5">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="1455" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A1455" s="11">
+        <v>45082.605555555558</v>
+      </c>
+      <c r="B1455" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1455" s="2" t="s">
+        <v>994</v>
+      </c>
+      <c r="D1455" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1455" s="4">
+        <v>102</v>
+      </c>
+      <c r="F1455" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1455" s="3"/>
+    </row>
+    <row r="1456" spans="1:16" ht="15.75" thickBot="1">
+      <c r="I1456" s="11"/>
+      <c r="J1456" s="2"/>
+      <c r="K1456" s="2"/>
+      <c r="L1456" s="3"/>
+      <c r="M1456" s="4"/>
+      <c r="N1456" s="2"/>
+      <c r="O1456" s="3"/>
+    </row>
+    <row r="1457" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A1457" s="11">
+        <v>45112.560416666667</v>
+      </c>
+      <c r="B1457" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K1380" s="2" t="s">
-        <v>971</v>
-      </c>
-      <c r="L1380" s="3">
+      <c r="C1457" s="2" t="s">
+        <v>993</v>
+      </c>
+      <c r="D1457" s="3">
         <v>-0.01</v>
       </c>
-      <c r="M1380" s="4">
-        <v>75</v>
-      </c>
-      <c r="N1380" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1380" s="5">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="P1380" s="2"/>
-    </row>
-    <row r="1381" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1381" s="2" t="s">
-        <v>972</v>
-      </c>
-      <c r="J1381" s="2" t="s">
+      <c r="E1457" s="4">
+        <v>30</v>
+      </c>
+      <c r="F1457" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1457" s="3">
+        <v>-0.22</v>
+      </c>
+      <c r="I1457" s="11"/>
+      <c r="J1457" s="2"/>
+      <c r="K1457" s="2"/>
+      <c r="L1457" s="5"/>
+      <c r="M1457" s="4"/>
+      <c r="N1457" s="2"/>
+      <c r="O1457" s="3"/>
+    </row>
+    <row r="1458" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A1458" s="11">
+        <v>45112.487500000003</v>
+      </c>
+      <c r="B1458" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K1381" s="2" t="s">
-        <v>971</v>
-      </c>
-      <c r="L1381" s="5">
+      <c r="C1458" s="2" t="s">
+        <v>993</v>
+      </c>
+      <c r="D1458" s="5">
         <v>0.01</v>
       </c>
-      <c r="M1381" s="4">
-        <v>68</v>
-      </c>
-      <c r="N1381" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1381" s="3"/>
-      <c r="P1381" s="2"/>
-    </row>
-    <row r="1382" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1382" s="2" t="s">
-        <v>973</v>
-      </c>
-      <c r="J1382" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1382" s="2" t="s">
-        <v>974</v>
-      </c>
-      <c r="L1382" s="3">
-        <v>-0.18</v>
-      </c>
-      <c r="M1382" s="4">
-        <v>5</v>
-      </c>
-      <c r="N1382" s="2" t="s">
+      <c r="E1458" s="4">
+        <v>52</v>
+      </c>
+      <c r="F1458" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1458" s="3"/>
+    </row>
+    <row r="1459" spans="1:15" ht="15.75" thickBot="1"/>
+    <row r="1460" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A1460" s="11">
+        <v>45112.693055555559</v>
+      </c>
+      <c r="B1460" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1460" s="2" t="s">
+        <v>992</v>
+      </c>
+      <c r="D1460" s="3">
+        <v>-0.02</v>
+      </c>
+      <c r="E1460" s="4">
+        <v>155</v>
+      </c>
+      <c r="F1460" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="O1382" s="5">
-        <v>0.35</v>
-      </c>
-      <c r="P1382" s="2"/>
-    </row>
-    <row r="1383" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1383" s="2" t="s">
-        <v>975</v>
-      </c>
-      <c r="J1383" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1383" s="2" t="s">
-        <v>974</v>
-      </c>
-      <c r="L1383" s="5">
-        <v>0.18</v>
-      </c>
-      <c r="M1383" s="4">
-        <v>3.05</v>
-      </c>
-      <c r="N1383" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1383" s="3"/>
-      <c r="P1383" s="2"/>
-    </row>
-    <row r="1384" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1384" s="2" t="s">
-        <v>976</v>
-      </c>
-      <c r="J1384" s="2" t="s">
+      <c r="G1460" s="5">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="1461" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A1461" s="11">
+        <v>45112.684027777781</v>
+      </c>
+      <c r="B1461" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="K1384" s="2" t="s">
-        <v>977</v>
-      </c>
-      <c r="L1384" s="3">
+      <c r="C1461" s="2" t="s">
+        <v>992</v>
+      </c>
+      <c r="D1461" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="E1461" s="4">
+        <v>117</v>
+      </c>
+      <c r="F1461" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1461" s="3"/>
+    </row>
+    <row r="1462" spans="1:15" ht="15.75" thickBot="1"/>
+    <row r="1463" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A1463" s="11">
+        <v>45112.872916666667</v>
+      </c>
+      <c r="B1463" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1463" s="2" t="s">
+        <v>991</v>
+      </c>
+      <c r="D1463" s="3">
+        <v>-0.02</v>
+      </c>
+      <c r="E1463" s="4">
+        <v>121</v>
+      </c>
+      <c r="F1463" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1463" s="5">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="1464" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A1464" s="11">
+        <v>45112.794444444444</v>
+      </c>
+      <c r="B1464" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1464" s="2" t="s">
+        <v>991</v>
+      </c>
+      <c r="D1464" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="E1464" s="4">
+        <v>117</v>
+      </c>
+      <c r="F1464" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1464" s="3"/>
+    </row>
+    <row r="1465" spans="1:15" ht="15.75" thickBot="1"/>
+    <row r="1466" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A1466" s="11">
+        <v>45143.856944444444</v>
+      </c>
+      <c r="B1466" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="C1466" s="2" t="s">
+        <v>990</v>
+      </c>
+      <c r="D1466" s="3">
         <v>-0.01</v>
       </c>
-      <c r="M1384" s="4">
-        <v>116</v>
-      </c>
-      <c r="N1384" s="2" t="s">
+      <c r="E1466" s="4">
+        <v>150</v>
+      </c>
+      <c r="F1466" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="O1384" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="P1384" s="2"/>
-    </row>
-    <row r="1385" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1385" s="2" t="s">
-        <v>978</v>
-      </c>
-      <c r="J1385" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1385" s="2" t="s">
-        <v>977</v>
-      </c>
-      <c r="L1385" s="3">
-        <v>-0.2</v>
-      </c>
-      <c r="M1385" s="4">
-        <v>4</v>
-      </c>
-      <c r="N1385" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O1385" s="5">
-        <v>0.26</v>
-      </c>
-      <c r="P1385" s="2"/>
-    </row>
-    <row r="1386" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1386" s="2" t="s">
-        <v>979</v>
-      </c>
-      <c r="J1386" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1386" s="2" t="s">
-        <v>977</v>
-      </c>
-      <c r="L1386" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="M1386" s="4">
-        <v>2.7</v>
-      </c>
-      <c r="N1386" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1386" s="3"/>
-      <c r="P1386" s="2"/>
-    </row>
-    <row r="1387" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1387" s="2" t="s">
-        <v>980</v>
-      </c>
-      <c r="J1387" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="K1387" s="2" t="s">
-        <v>977</v>
-      </c>
-      <c r="L1387" s="5">
+      <c r="G1466" s="5">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="1467" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A1467" s="11">
+        <v>45143.84097222222</v>
+      </c>
+      <c r="B1467" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="C1467" s="2" t="s">
+        <v>990</v>
+      </c>
+      <c r="D1467" s="5">
         <v>0.01</v>
       </c>
-      <c r="M1387" s="4">
-        <v>106</v>
-      </c>
-      <c r="N1387" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1387" s="3"/>
-      <c r="P1387" s="2"/>
-    </row>
-    <row r="1388" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1388" s="2" t="s">
-        <v>981</v>
-      </c>
-      <c r="J1388" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="K1388" s="2" t="s">
-        <v>982</v>
-      </c>
-      <c r="L1388" s="3">
-        <v>-0.01</v>
-      </c>
-      <c r="M1388" s="4">
-        <v>142</v>
-      </c>
-      <c r="N1388" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O1388" s="5">
-        <v>0.19</v>
-      </c>
-      <c r="P1388" s="2"/>
-    </row>
-    <row r="1389" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1389" s="2" t="s">
-        <v>983</v>
-      </c>
-      <c r="J1389" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="K1389" s="2" t="s">
-        <v>982</v>
-      </c>
-      <c r="L1389" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="M1389" s="4">
-        <v>123</v>
-      </c>
-      <c r="N1389" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1389" s="3"/>
-      <c r="P1389" s="2"/>
-    </row>
-    <row r="1390" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1390" s="2" t="s">
-        <v>984</v>
-      </c>
-      <c r="J1390" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="K1390" s="2" t="s">
-        <v>985</v>
-      </c>
-      <c r="L1390" s="3">
-        <v>-0.01</v>
-      </c>
-      <c r="M1390" s="4">
-        <v>25</v>
-      </c>
-      <c r="N1390" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1390" s="3">
-        <v>-0.88</v>
-      </c>
-      <c r="P1390" s="2"/>
-    </row>
-    <row r="1391" spans="9:16" ht="15.75" thickBot="1">
-      <c r="P1391" s="2"/>
-    </row>
-    <row r="1392" spans="9:16" ht="15.75" thickBot="1">
-      <c r="I1392" s="2" t="s">
-        <v>988</v>
-      </c>
-      <c r="J1392" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="K1392" s="2" t="s">
-        <v>985</v>
-      </c>
-      <c r="L1392" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="M1392" s="4">
-        <v>113</v>
-      </c>
-      <c r="N1392" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1392" s="3"/>
-      <c r="P1392" s="2"/>
-    </row>
-    <row r="1393" spans="15:16" ht="15.75" thickBot="1">
-      <c r="O1393" s="3"/>
-      <c r="P1393" s="2"/>
+      <c r="E1467" s="4">
+        <v>36</v>
+      </c>
+      <c r="F1467" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1467" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new season 2023 2024
</commit_message>
<xml_diff>
--- a/spreadex.xlsx
+++ b/spreadex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kovan\FDAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E90A2E-9583-4F12-8252-429327807227}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097EFEAA-9A9A-49D0-BD7F-3E1322439FCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="802" xr2:uid="{8365F371-5EDF-4C19-B0B3-71E11A5B2E12}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5015" uniqueCount="1079">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5111" uniqueCount="1103">
   <si>
     <t>24/11/2022 20:55</t>
   </si>
@@ -3282,6 +3282,78 @@
   </si>
   <si>
     <t>Juventus v Sevilla</t>
+  </si>
+  <si>
+    <t>19/06/2023 21:49</t>
+  </si>
+  <si>
+    <t>France v Greece</t>
+  </si>
+  <si>
+    <t>19/06/2023 19:49</t>
+  </si>
+  <si>
+    <t>Spezia v Verona</t>
+  </si>
+  <si>
+    <t>14/08/2023 20:14</t>
+  </si>
+  <si>
+    <t>Man Utd v Wolves</t>
+  </si>
+  <si>
+    <t>14/08/2023 20:06</t>
+  </si>
+  <si>
+    <t>Newcastle v Aston Villa</t>
+  </si>
+  <si>
+    <t>Arsenal v Nottingham Forest</t>
+  </si>
+  <si>
+    <t>Burnley v Man City</t>
+  </si>
+  <si>
+    <t>Leicester v Coventry</t>
+  </si>
+  <si>
+    <t>Celtic v Ross County</t>
+  </si>
+  <si>
+    <t>Paderborn v Osnabruck</t>
+  </si>
+  <si>
+    <t>30/07/2023 14:27</t>
+  </si>
+  <si>
+    <t>30/07/2023 13:03</t>
+  </si>
+  <si>
+    <t>29/07/2023 21:24</t>
+  </si>
+  <si>
+    <t>Dusseldorf v Hertha BSC</t>
+  </si>
+  <si>
+    <t>29/07/2023 19:35</t>
+  </si>
+  <si>
+    <t>28/07/2023 19:52</t>
+  </si>
+  <si>
+    <t>Hamburg v Schalke</t>
+  </si>
+  <si>
+    <t>28/07/2023 19:42</t>
+  </si>
+  <si>
+    <t>15/07/2023 16:51</t>
+  </si>
+  <si>
+    <t>Chesterfield v Sheff Utd</t>
+  </si>
+  <si>
+    <t>15/07/2023 16:35</t>
   </si>
 </sst>
 </file>
@@ -3850,13 +3922,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B2ACDE7-BC8B-432A-9773-10E95E9E94B1}">
-  <dimension ref="A1:V1507"/>
+  <dimension ref="A1:V1556"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B1465" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B1522" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B1482" sqref="B1482"/>
+      <selection pane="bottomRight" activeCell="O1561" sqref="O1561"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -28359,27 +28431,6 @@
       <c r="Q1467" s="1"/>
     </row>
     <row r="1468" spans="1:17" ht="15.75" thickBot="1">
-      <c r="J1468" s="11">
-        <v>45022.779861111114</v>
-      </c>
-      <c r="K1468" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1468" s="2" t="s">
-        <v>1024</v>
-      </c>
-      <c r="M1468" s="3">
-        <v>-0.19</v>
-      </c>
-      <c r="N1468" s="4">
-        <v>2.7</v>
-      </c>
-      <c r="O1468" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="P1468" s="3">
-        <v>-0.05</v>
-      </c>
       <c r="Q1468" s="2"/>
     </row>
     <row r="1469" spans="1:17" ht="15.75" thickBot="1">
@@ -28404,25 +28455,6 @@
       <c r="G1469" s="5">
         <v>0</v>
       </c>
-      <c r="J1469" s="11">
-        <v>45022.720138888886</v>
-      </c>
-      <c r="K1469" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1469" s="2" t="s">
-        <v>1024</v>
-      </c>
-      <c r="M1469" s="5">
-        <v>0.19</v>
-      </c>
-      <c r="N1469" s="4">
-        <v>2.95</v>
-      </c>
-      <c r="O1469" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1469" s="3"/>
       <c r="Q1469" s="2"/>
     </row>
     <row r="1470" spans="1:17" ht="15.75" thickBot="1">
@@ -28445,49 +28477,9 @@
         <v>5</v>
       </c>
       <c r="G1470" s="1"/>
-      <c r="J1470" s="11">
-        <v>44963.875</v>
-      </c>
-      <c r="K1470" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1470" s="2" t="s">
-        <v>1025</v>
-      </c>
-      <c r="M1470" s="3">
-        <v>-0.19</v>
-      </c>
-      <c r="N1470" s="4">
-        <v>2.8</v>
-      </c>
-      <c r="O1470" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="P1470" s="5">
-        <v>0.1</v>
-      </c>
       <c r="Q1470" s="2"/>
     </row>
     <row r="1471" spans="1:17" ht="15.75" thickBot="1">
-      <c r="J1471" s="11">
-        <v>44963.838888888888</v>
-      </c>
-      <c r="K1471" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1471" s="2" t="s">
-        <v>1025</v>
-      </c>
-      <c r="M1471" s="5">
-        <v>0.19</v>
-      </c>
-      <c r="N1471" s="4">
-        <v>2.25</v>
-      </c>
-      <c r="O1471" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1471" s="3"/>
       <c r="Q1471" s="2"/>
     </row>
     <row r="1472" spans="1:17" ht="15.75" thickBot="1">
@@ -28512,27 +28504,6 @@
       <c r="G1472" s="3">
         <v>-0.45</v>
       </c>
-      <c r="J1472" s="2" t="s">
-        <v>1026</v>
-      </c>
-      <c r="K1472" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="L1472" s="2" t="s">
-        <v>1027</v>
-      </c>
-      <c r="M1472" s="3">
-        <v>-0.01</v>
-      </c>
-      <c r="N1472" s="4">
-        <v>25</v>
-      </c>
-      <c r="O1472" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="P1472" s="3">
-        <v>-0.82</v>
-      </c>
       <c r="Q1472" s="2"/>
     </row>
     <row r="1473" spans="1:17" ht="15.75" thickBot="1">
@@ -28555,49 +28526,9 @@
         <v>5</v>
       </c>
       <c r="G1473" s="3"/>
-      <c r="J1473" s="2" t="s">
-        <v>1028</v>
-      </c>
-      <c r="K1473" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="L1473" s="2" t="s">
-        <v>1027</v>
-      </c>
-      <c r="M1473" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="N1473" s="4">
-        <v>107</v>
-      </c>
-      <c r="O1473" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1473" s="3"/>
       <c r="Q1473" s="2"/>
     </row>
     <row r="1474" spans="1:17" ht="15.75" thickBot="1">
-      <c r="J1474" s="2" t="s">
-        <v>1029</v>
-      </c>
-      <c r="K1474" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1474" s="2" t="s">
-        <v>1030</v>
-      </c>
-      <c r="M1474" s="3">
-        <v>-0.19</v>
-      </c>
-      <c r="N1474" s="4">
-        <v>2</v>
-      </c>
-      <c r="O1474" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="P1474" s="3">
-        <v>-0.23</v>
-      </c>
       <c r="Q1474" s="2"/>
     </row>
     <row r="1475" spans="1:17" ht="15.75" thickBot="1">
@@ -28622,25 +28553,6 @@
       <c r="G1475" s="5">
         <v>0.05</v>
       </c>
-      <c r="J1475" s="2" t="s">
-        <v>1031</v>
-      </c>
-      <c r="K1475" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1475" s="2" t="s">
-        <v>1030</v>
-      </c>
-      <c r="M1475" s="5">
-        <v>0.19</v>
-      </c>
-      <c r="N1475" s="4">
-        <v>3.2</v>
-      </c>
-      <c r="O1475" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1475" s="3"/>
       <c r="Q1475" s="2"/>
     </row>
     <row r="1476" spans="1:17" ht="15.75" thickBot="1">
@@ -28663,620 +28575,1469 @@
         <v>5</v>
       </c>
       <c r="G1476" s="3"/>
-      <c r="J1476" s="2" t="s">
+      <c r="Q1476" s="2"/>
+    </row>
+    <row r="1477" spans="1:17" ht="15.75" thickBot="1">
+      <c r="Q1477" s="2"/>
+    </row>
+    <row r="1478" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1478" s="2" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B1478" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1478" s="2" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D1478" s="3">
+        <v>-0.5</v>
+      </c>
+      <c r="E1478" s="4">
+        <v>2.25</v>
+      </c>
+      <c r="F1478" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1478" s="5">
+        <v>0.13</v>
+      </c>
+      <c r="Q1478" s="2"/>
+    </row>
+    <row r="1479" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1479" s="2" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B1479" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1479" s="2" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D1479" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E1479" s="4">
+        <v>2</v>
+      </c>
+      <c r="F1479" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1479" s="3"/>
+      <c r="Q1479" s="2"/>
+    </row>
+    <row r="1480" spans="1:17" ht="15.75" thickBot="1">
+      <c r="Q1480" s="2"/>
+    </row>
+    <row r="1481" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1481" s="2" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B1481" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1481" s="2" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D1481" s="3">
+        <v>-0.05</v>
+      </c>
+      <c r="E1481" s="4">
+        <v>139</v>
+      </c>
+      <c r="F1481" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1481" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J1481" s="1"/>
+      <c r="K1481" s="1"/>
+      <c r="L1481" s="1"/>
+      <c r="M1481" s="1"/>
+      <c r="N1481" s="1"/>
+      <c r="O1481" s="1"/>
+      <c r="P1481" s="1"/>
+      <c r="Q1481" s="1"/>
+    </row>
+    <row r="1482" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1482" s="2" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B1482" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1482" s="2" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D1482" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="E1482" s="4">
+        <v>117</v>
+      </c>
+      <c r="F1482" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1482" s="3"/>
+      <c r="Q1482" s="2"/>
+    </row>
+    <row r="1483" spans="1:17" ht="15.75" thickBot="1">
+      <c r="Q1483" s="2"/>
+    </row>
+    <row r="1484" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1484" s="2" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B1484" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1484" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="D1484" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1484" s="4">
+        <v>147</v>
+      </c>
+      <c r="F1484" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1484" s="5">
+        <v>0.35</v>
+      </c>
+      <c r="Q1484" s="2"/>
+    </row>
+    <row r="1485" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1485" s="2" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B1485" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1485" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="D1485" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1485" s="4">
+        <v>112</v>
+      </c>
+      <c r="F1485" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1485" s="3"/>
+      <c r="Q1485" s="2"/>
+    </row>
+    <row r="1486" spans="1:17" ht="15.75" thickBot="1">
+      <c r="Q1486" s="2"/>
+    </row>
+    <row r="1487" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1487" s="2" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B1487" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1487" s="2" t="s">
+        <v>1061</v>
+      </c>
+      <c r="D1487" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1487" s="4">
+        <v>131</v>
+      </c>
+      <c r="F1487" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1487" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="Q1487" s="2"/>
+    </row>
+    <row r="1488" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1488" s="2" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B1488" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1488" s="2" t="s">
+        <v>1061</v>
+      </c>
+      <c r="D1488" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1488" s="4">
+        <v>108</v>
+      </c>
+      <c r="F1488" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1488" s="3"/>
+      <c r="Q1488" s="2"/>
+    </row>
+    <row r="1489" spans="1:17" ht="15.75" thickBot="1">
+      <c r="Q1489" s="2"/>
+    </row>
+    <row r="1490" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1490" s="2" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B1490" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="C1490" s="2" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1490" s="3">
+        <v>-0.02</v>
+      </c>
+      <c r="E1490" s="4">
+        <v>27</v>
+      </c>
+      <c r="F1490" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1490" s="3">
+        <v>-0.84</v>
+      </c>
+      <c r="Q1490" s="2"/>
+    </row>
+    <row r="1491" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1491" s="2" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B1491" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="C1491" s="2" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1491" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="E1491" s="4">
+        <v>69</v>
+      </c>
+      <c r="F1491" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1491" s="3"/>
+      <c r="Q1491" s="2"/>
+    </row>
+    <row r="1492" spans="1:17" ht="15.75" thickBot="1">
+      <c r="Q1492" s="2"/>
+    </row>
+    <row r="1493" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1493" s="2" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B1493" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1493" s="2" t="s">
+        <v>1055</v>
+      </c>
+      <c r="D1493" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="E1493" s="4">
+        <v>2.25</v>
+      </c>
+      <c r="F1493" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1493" s="5">
+        <v>0.06</v>
+      </c>
+      <c r="Q1493" s="2"/>
+    </row>
+    <row r="1494" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1494" s="2" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B1494" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1494" s="2" t="s">
+        <v>1055</v>
+      </c>
+      <c r="D1494" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="E1494" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="F1494" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1494" s="3"/>
+      <c r="Q1494" s="2"/>
+    </row>
+    <row r="1495" spans="1:17" ht="15.75" thickBot="1">
+      <c r="Q1495" s="2"/>
+    </row>
+    <row r="1496" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1496" s="2" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B1496" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1496" s="2" t="s">
+        <v>1052</v>
+      </c>
+      <c r="D1496" s="3">
+        <v>-0.5</v>
+      </c>
+      <c r="E1496" s="4">
+        <v>2</v>
+      </c>
+      <c r="F1496" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1496" s="3">
+        <v>-0.5</v>
+      </c>
+      <c r="Q1496" s="2"/>
+    </row>
+    <row r="1497" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1497" s="2" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B1497" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1497" s="2" t="s">
+        <v>1052</v>
+      </c>
+      <c r="D1497" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E1497" s="4">
+        <v>3</v>
+      </c>
+      <c r="F1497" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1497" s="3"/>
+      <c r="Q1497" s="2"/>
+    </row>
+    <row r="1498" spans="1:17" ht="15.75" thickBot="1">
+      <c r="Q1498" s="2"/>
+    </row>
+    <row r="1499" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1499" s="2" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B1499" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1499" s="2" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D1499" s="3">
+        <v>-0.2</v>
+      </c>
+      <c r="E1499" s="4">
+        <v>3.25</v>
+      </c>
+      <c r="F1499" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1499" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="Q1499" s="2"/>
+    </row>
+    <row r="1500" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1500" s="2" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B1500" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1500" s="2" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D1500" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="E1500" s="4">
+        <v>2.75</v>
+      </c>
+      <c r="F1500" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1500" s="3"/>
+      <c r="Q1500" s="2"/>
+    </row>
+    <row r="1501" spans="1:17" ht="15.75" thickBot="1">
+      <c r="Q1501" s="2"/>
+    </row>
+    <row r="1502" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1502" s="2" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B1502" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1502" s="2" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D1502" s="3">
+        <v>-0.03</v>
+      </c>
+      <c r="E1502" s="4">
+        <v>163</v>
+      </c>
+      <c r="F1502" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1502" s="5">
+        <v>1.35</v>
+      </c>
+      <c r="Q1502" s="2"/>
+    </row>
+    <row r="1503" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1503" s="2" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B1503" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1503" s="2" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D1503" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="E1503" s="4">
+        <v>118</v>
+      </c>
+      <c r="F1503" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1503" s="3"/>
+      <c r="Q1503" s="2"/>
+    </row>
+    <row r="1504" spans="1:17" ht="15.75" thickBot="1">
+      <c r="Q1504" s="2"/>
+    </row>
+    <row r="1505" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1505" s="2" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B1505" s="2" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C1505" s="2" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D1505" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1505" s="4">
+        <v>200</v>
+      </c>
+      <c r="F1505" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1505" s="3">
+        <v>-1.9</v>
+      </c>
+      <c r="Q1505" s="2"/>
+    </row>
+    <row r="1506" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1506" s="2" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B1506" s="2" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C1506" s="2" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D1506" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1506" s="4">
+        <v>390</v>
+      </c>
+      <c r="F1506" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1506" s="3"/>
+      <c r="Q1506" s="2"/>
+    </row>
+    <row r="1507" spans="1:17" ht="15.75" thickBot="1">
+      <c r="Q1507" s="1"/>
+    </row>
+    <row r="1508" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1508" s="2" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B1508" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1508" s="2" t="s">
+        <v>1039</v>
+      </c>
+      <c r="D1508" s="3">
+        <v>-0.05</v>
+      </c>
+      <c r="E1508" s="4">
+        <v>20</v>
+      </c>
+      <c r="F1508" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1508" s="3">
+        <v>-1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="1509" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1509" s="2" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B1509" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1509" s="2" t="s">
+        <v>1039</v>
+      </c>
+      <c r="D1509" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="E1509" s="4">
+        <v>43</v>
+      </c>
+      <c r="F1509" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1509" s="3"/>
+    </row>
+    <row r="1510" spans="1:17" ht="15.75" thickBot="1"/>
+    <row r="1511" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1511" s="2" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B1511" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1511" s="2" t="s">
+        <v>1036</v>
+      </c>
+      <c r="D1511" s="3">
+        <v>-0.05</v>
+      </c>
+      <c r="E1511" s="4">
+        <v>165</v>
+      </c>
+      <c r="F1511" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1511" s="5">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="1512" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1512" s="2" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B1512" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1512" s="2" t="s">
+        <v>1036</v>
+      </c>
+      <c r="D1512" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="E1512" s="4">
+        <v>117</v>
+      </c>
+      <c r="F1512" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1512" s="3"/>
+    </row>
+    <row r="1513" spans="1:17" ht="15.75" thickBot="1"/>
+    <row r="1514" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1514" s="2" t="s">
         <v>1032</v>
       </c>
-      <c r="K1476" s="2" t="s">
+      <c r="B1514" s="2" t="s">
         <v>813</v>
       </c>
-      <c r="L1476" s="2" t="s">
+      <c r="C1514" s="2" t="s">
         <v>1033</v>
       </c>
-      <c r="M1476" s="3">
+      <c r="D1514" s="3">
         <v>-0.05</v>
       </c>
-      <c r="N1476" s="4">
+      <c r="E1514" s="4">
         <v>0</v>
       </c>
-      <c r="O1476" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="P1476" s="3">
+      <c r="F1514" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1514" s="3">
         <v>-3.65</v>
       </c>
-      <c r="Q1476" s="2"/>
-    </row>
-    <row r="1477" spans="1:17" ht="15.75" thickBot="1">
-      <c r="J1477" s="2" t="s">
+    </row>
+    <row r="1515" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1515" s="2" t="s">
         <v>1034</v>
       </c>
-      <c r="K1477" s="2" t="s">
+      <c r="B1515" s="2" t="s">
         <v>813</v>
       </c>
-      <c r="L1477" s="2" t="s">
+      <c r="C1515" s="2" t="s">
         <v>1033</v>
       </c>
-      <c r="M1477" s="5">
+      <c r="D1515" s="5">
         <v>0.05</v>
       </c>
-      <c r="N1477" s="4">
+      <c r="E1515" s="4">
         <v>73</v>
       </c>
-      <c r="O1477" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1477" s="3"/>
-      <c r="Q1477" s="2"/>
-    </row>
-    <row r="1478" spans="1:17" ht="15.75" thickBot="1">
-      <c r="J1478" s="2" t="s">
-        <v>1035</v>
-      </c>
-      <c r="K1478" s="2" t="s">
+      <c r="F1515" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1515" s="3"/>
+    </row>
+    <row r="1516" spans="1:17" ht="15.75" thickBot="1"/>
+    <row r="1517" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1517" s="2" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B1517" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1517" s="2" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D1517" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="E1517" s="4">
+        <v>2</v>
+      </c>
+      <c r="F1517" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1517" s="3">
+        <v>-0.23</v>
+      </c>
+    </row>
+    <row r="1518" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1518" s="2" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B1518" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1518" s="2" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D1518" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="E1518" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="F1518" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1518" s="3"/>
+    </row>
+    <row r="1519" spans="1:17" ht="15.75" thickBot="1"/>
+    <row r="1520" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1520" s="2" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B1520" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L1478" s="2" t="s">
-        <v>1036</v>
-      </c>
-      <c r="M1478" s="3">
+      <c r="C1520" s="2" t="s">
+        <v>1027</v>
+      </c>
+      <c r="D1520" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1520" s="4">
+        <v>25</v>
+      </c>
+      <c r="F1520" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1520" s="3">
+        <v>-0.82</v>
+      </c>
+    </row>
+    <row r="1521" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1521" s="2" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B1521" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1521" s="2" t="s">
+        <v>1027</v>
+      </c>
+      <c r="D1521" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1521" s="4">
+        <v>107</v>
+      </c>
+      <c r="F1521" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1521" s="3"/>
+    </row>
+    <row r="1522" spans="1:17" ht="15.75" thickBot="1"/>
+    <row r="1523" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1523" s="11">
+        <v>44963.875</v>
+      </c>
+      <c r="B1523" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1523" s="2" t="s">
+        <v>1025</v>
+      </c>
+      <c r="D1523" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="E1523" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="F1523" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1523" s="5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="1524" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1524" s="11">
+        <v>44963.838888888888</v>
+      </c>
+      <c r="B1524" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1524" s="2" t="s">
+        <v>1025</v>
+      </c>
+      <c r="D1524" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="E1524" s="4">
+        <v>2.25</v>
+      </c>
+      <c r="F1524" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1524" s="3"/>
+    </row>
+    <row r="1525" spans="1:17" ht="15.75" thickBot="1"/>
+    <row r="1526" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1526" s="11">
+        <v>45022.779861111114</v>
+      </c>
+      <c r="B1526" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1526" s="2" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D1526" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="E1526" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="F1526" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1526" s="3">
         <v>-0.05</v>
       </c>
-      <c r="N1478" s="4">
-        <v>165</v>
-      </c>
-      <c r="O1478" s="2" t="s">
+    </row>
+    <row r="1527" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1527" s="11">
+        <v>45022.720138888886</v>
+      </c>
+      <c r="B1527" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1527" s="2" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D1527" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="E1527" s="4">
+        <v>2.95</v>
+      </c>
+      <c r="F1527" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1527" s="3"/>
+    </row>
+    <row r="1528" spans="1:17" ht="15.75" thickBot="1"/>
+    <row r="1529" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1529" s="11">
+        <v>45236.885416666664</v>
+      </c>
+      <c r="B1529" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1529" s="2" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D1529" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E1529" s="4">
+        <v>119</v>
+      </c>
+      <c r="F1529" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="P1478" s="5">
-        <v>2.4</v>
-      </c>
-      <c r="Q1478" s="2"/>
-    </row>
-    <row r="1479" spans="1:17" ht="15.75" thickBot="1">
-      <c r="J1479" s="2" t="s">
-        <v>1037</v>
-      </c>
-      <c r="K1479" s="2" t="s">
+      <c r="G1529" s="5">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="1530" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1530" s="11">
+        <v>45236.824999999997</v>
+      </c>
+      <c r="B1530" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L1479" s="2" t="s">
-        <v>1036</v>
-      </c>
-      <c r="M1479" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="N1479" s="4">
-        <v>117</v>
-      </c>
-      <c r="O1479" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1479" s="3"/>
-      <c r="Q1479" s="2"/>
-    </row>
-    <row r="1480" spans="1:17" ht="15.75" thickBot="1">
-      <c r="J1480" s="2" t="s">
-        <v>1038</v>
-      </c>
-      <c r="K1480" s="2" t="s">
+      <c r="C1530" s="2" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D1530" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E1530" s="4">
+        <v>101</v>
+      </c>
+      <c r="F1530" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1530" s="3"/>
+    </row>
+    <row r="1531" spans="1:17" ht="15.75" thickBot="1"/>
+    <row r="1532" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1532" s="2" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B1532" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1532" s="2" t="s">
+        <v>1080</v>
+      </c>
+      <c r="D1532" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="E1532" s="4">
+        <v>1</v>
+      </c>
+      <c r="F1532" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1532" s="3">
+        <v>-0.35</v>
+      </c>
+      <c r="J1532" s="1"/>
+      <c r="K1532" s="1"/>
+      <c r="L1532" s="1"/>
+      <c r="M1532" s="1"/>
+      <c r="N1532" s="1"/>
+      <c r="O1532" s="1"/>
+      <c r="P1532" s="1"/>
+      <c r="Q1532" s="1"/>
+    </row>
+    <row r="1533" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1533" s="2" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B1533" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1533" s="2" t="s">
+        <v>1080</v>
+      </c>
+      <c r="D1533" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="E1533" s="4">
+        <v>2.85</v>
+      </c>
+      <c r="F1533" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1533" s="3"/>
+      <c r="J1533" s="2" t="s">
+        <v>1083</v>
+      </c>
+      <c r="K1533" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="L1533" s="2" t="s">
+        <v>1084</v>
+      </c>
+      <c r="M1533" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="N1533" s="4">
+        <v>159</v>
+      </c>
+      <c r="O1533" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="P1533" s="5">
+        <v>0.37</v>
+      </c>
+      <c r="Q1533" s="2"/>
+    </row>
+    <row r="1534" spans="1:17" ht="15.75" thickBot="1">
+      <c r="J1534" s="2" t="s">
+        <v>1085</v>
+      </c>
+      <c r="K1534" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="L1534" s="2" t="s">
+        <v>1084</v>
+      </c>
+      <c r="M1534" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="N1534" s="4">
+        <v>122</v>
+      </c>
+      <c r="O1534" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1534" s="3"/>
+      <c r="Q1534" s="2"/>
+    </row>
+    <row r="1535" spans="1:17" ht="15.75" thickBot="1">
+      <c r="J1535" s="11">
+        <v>45268.81527777778</v>
+      </c>
+      <c r="K1535" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="L1535" s="2" t="s">
+        <v>1086</v>
+      </c>
+      <c r="M1535" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="N1535" s="4">
+        <v>121</v>
+      </c>
+      <c r="O1535" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1535" s="3">
+        <v>-0.11</v>
+      </c>
+      <c r="Q1535" s="2"/>
+    </row>
+    <row r="1536" spans="1:17" ht="15.75" thickBot="1">
+      <c r="J1536" s="11">
+        <v>45268.730555555558</v>
+      </c>
+      <c r="K1536" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="L1536" s="2" t="s">
+        <v>1086</v>
+      </c>
+      <c r="M1536" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="N1536" s="4">
+        <v>132</v>
+      </c>
+      <c r="O1536" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1536" s="3"/>
+      <c r="Q1536" s="2"/>
+    </row>
+    <row r="1537" spans="10:17" ht="15.75" thickBot="1">
+      <c r="J1537" s="11">
+        <v>45268.56527777778</v>
+      </c>
+      <c r="K1537" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="L1537" s="2" t="s">
+        <v>1087</v>
+      </c>
+      <c r="M1537" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="N1537" s="4">
+        <v>88</v>
+      </c>
+      <c r="O1537" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="P1537" s="5">
+        <v>0.37</v>
+      </c>
+      <c r="Q1537" s="2"/>
+    </row>
+    <row r="1538" spans="10:17" ht="15.75" thickBot="1">
+      <c r="J1538" s="11">
+        <v>45268.552083333336</v>
+      </c>
+      <c r="K1538" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="L1538" s="2" t="s">
+        <v>1087</v>
+      </c>
+      <c r="M1538" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="N1538" s="4">
+        <v>51</v>
+      </c>
+      <c r="O1538" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1538" s="3"/>
+      <c r="Q1538" s="2"/>
+    </row>
+    <row r="1539" spans="10:17" ht="15.75" thickBot="1">
+      <c r="J1539" s="11">
+        <v>45238.917361111111</v>
+      </c>
+      <c r="K1539" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L1480" s="2" t="s">
-        <v>1039</v>
-      </c>
-      <c r="M1480" s="3">
-        <v>-0.05</v>
-      </c>
-      <c r="N1480" s="4">
+      <c r="L1539" s="2" t="s">
+        <v>1088</v>
+      </c>
+      <c r="M1539" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="N1539" s="4">
+        <v>25</v>
+      </c>
+      <c r="O1539" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1539" s="3">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="Q1539" s="2"/>
+    </row>
+    <row r="1540" spans="10:17" ht="15.75" thickBot="1">
+      <c r="J1540" s="11">
+        <v>45238.84097222222</v>
+      </c>
+      <c r="K1540" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O1480" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="P1480" s="3">
-        <v>-1.1499999999999999</v>
-      </c>
-      <c r="Q1480" s="2"/>
-    </row>
-    <row r="1481" spans="1:17" ht="15.75" thickBot="1">
-      <c r="J1481" s="2" t="s">
-        <v>1040</v>
-      </c>
-      <c r="K1481" s="2" t="s">
+      <c r="L1540" s="2" t="s">
+        <v>1088</v>
+      </c>
+      <c r="M1540" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="N1540" s="4">
+        <v>39</v>
+      </c>
+      <c r="O1540" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1540" s="3"/>
+      <c r="Q1540" s="2"/>
+    </row>
+    <row r="1541" spans="10:17" ht="15.75" thickBot="1">
+      <c r="J1541" s="11">
+        <v>45085.754166666666</v>
+      </c>
+      <c r="K1541" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="L1541" s="2" t="s">
+        <v>1022</v>
+      </c>
+      <c r="M1541" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="N1541" s="4">
+        <v>0</v>
+      </c>
+      <c r="O1541" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1541" s="3">
+        <v>-0.2</v>
+      </c>
+      <c r="Q1541" s="2"/>
+    </row>
+    <row r="1542" spans="10:17" ht="15.75" thickBot="1">
+      <c r="J1542" s="11">
+        <v>45085.686805555553</v>
+      </c>
+      <c r="K1542" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="L1542" s="2" t="s">
+        <v>1022</v>
+      </c>
+      <c r="M1542" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="N1542" s="4">
         <v>20</v>
       </c>
-      <c r="L1481" s="2" t="s">
-        <v>1039</v>
-      </c>
-      <c r="M1481" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="N1481" s="4">
-        <v>43</v>
-      </c>
-      <c r="O1481" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1481" s="3"/>
-      <c r="Q1481" s="2"/>
-    </row>
-    <row r="1482" spans="1:17" ht="15.75" thickBot="1">
-      <c r="J1482" s="2" t="s">
-        <v>1041</v>
-      </c>
-      <c r="K1482" s="2" t="s">
-        <v>1042</v>
-      </c>
-      <c r="L1482" s="2" t="s">
-        <v>1043</v>
-      </c>
-      <c r="M1482" s="3">
-        <v>-0.01</v>
-      </c>
-      <c r="N1482" s="4">
-        <v>200</v>
-      </c>
-      <c r="O1482" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="P1482" s="3">
-        <v>-1.9</v>
-      </c>
-      <c r="Q1482" s="2"/>
-    </row>
-    <row r="1483" spans="1:17" ht="15.75" thickBot="1">
-      <c r="J1483" s="2" t="s">
-        <v>1044</v>
-      </c>
-      <c r="K1483" s="2" t="s">
-        <v>1042</v>
-      </c>
-      <c r="L1483" s="2" t="s">
-        <v>1043</v>
-      </c>
-      <c r="M1483" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="N1483" s="4">
-        <v>390</v>
-      </c>
-      <c r="O1483" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1483" s="3"/>
-      <c r="Q1483" s="2"/>
-    </row>
-    <row r="1484" spans="1:17" ht="15.75" thickBot="1">
-      <c r="J1484" s="2" t="s">
-        <v>1045</v>
-      </c>
-      <c r="K1484" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="L1484" s="2" t="s">
-        <v>1046</v>
-      </c>
-      <c r="M1484" s="3">
-        <v>-0.03</v>
-      </c>
-      <c r="N1484" s="4">
-        <v>163</v>
-      </c>
-      <c r="O1484" s="2" t="s">
+      <c r="O1542" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1542" s="3"/>
+      <c r="Q1542" s="2"/>
+    </row>
+    <row r="1543" spans="10:17" ht="15.75" thickBot="1">
+      <c r="J1543" s="11">
+        <v>45085.575694444444</v>
+      </c>
+      <c r="K1543" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1543" s="2" t="s">
+        <v>1089</v>
+      </c>
+      <c r="M1543" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="N1543" s="4">
+        <v>3.25</v>
+      </c>
+      <c r="O1543" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="P1484" s="5">
-        <v>1.35</v>
-      </c>
-      <c r="Q1484" s="2"/>
-    </row>
-    <row r="1485" spans="1:17" ht="15.75" thickBot="1">
-      <c r="J1485" s="2" t="s">
-        <v>1047</v>
-      </c>
-      <c r="K1485" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="L1485" s="2" t="s">
-        <v>1046</v>
-      </c>
-      <c r="M1485" s="5">
-        <v>0.03</v>
-      </c>
-      <c r="N1485" s="4">
-        <v>118</v>
-      </c>
-      <c r="O1485" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1485" s="3"/>
-      <c r="Q1485" s="2"/>
-    </row>
-    <row r="1486" spans="1:17" ht="15.75" thickBot="1">
-      <c r="J1486" s="2" t="s">
-        <v>1048</v>
-      </c>
-      <c r="K1486" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1486" s="2" t="s">
-        <v>1049</v>
-      </c>
-      <c r="M1486" s="3">
+      <c r="P1543" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="Q1543" s="2"/>
+    </row>
+    <row r="1544" spans="10:17" ht="15.75" thickBot="1">
+      <c r="J1544" s="11">
+        <v>45085.525694444441</v>
+      </c>
+      <c r="K1544" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1544" s="2" t="s">
+        <v>1089</v>
+      </c>
+      <c r="M1544" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="N1544" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="O1544" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1544" s="3"/>
+      <c r="Q1544" s="2"/>
+    </row>
+    <row r="1545" spans="10:17" ht="15.75" thickBot="1">
+      <c r="J1545" s="11">
+        <v>45054.603472222225</v>
+      </c>
+      <c r="K1545" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1545" s="2" t="s">
+        <v>1090</v>
+      </c>
+      <c r="M1545" s="3">
+        <v>-0.4</v>
+      </c>
+      <c r="N1545" s="4">
+        <v>6</v>
+      </c>
+      <c r="O1545" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1545" s="5">
+        <v>0.84</v>
+      </c>
+      <c r="Q1545" s="2"/>
+    </row>
+    <row r="1546" spans="10:17" ht="15.75" thickBot="1">
+      <c r="J1546" s="11">
+        <v>45054.529166666667</v>
+      </c>
+      <c r="K1546" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1546" s="2" t="s">
+        <v>1090</v>
+      </c>
+      <c r="M1546" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="N1546" s="4">
+        <v>3.9</v>
+      </c>
+      <c r="O1546" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1546" s="3"/>
+      <c r="Q1546" s="2"/>
+    </row>
+    <row r="1547" spans="10:17" ht="15.75" thickBot="1">
+      <c r="J1547" s="11">
+        <v>45024.808333333334</v>
+      </c>
+      <c r="K1547" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1547" s="2" t="s">
+        <v>1091</v>
+      </c>
+      <c r="M1547" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="N1547" s="4">
+        <v>2</v>
+      </c>
+      <c r="O1547" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1547" s="3">
+        <v>-0.27</v>
+      </c>
+      <c r="Q1547" s="2"/>
+    </row>
+    <row r="1548" spans="10:17" ht="15.75" thickBot="1">
+      <c r="J1548" s="11">
+        <v>45024.732638888891</v>
+      </c>
+      <c r="K1548" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1548" s="2" t="s">
+        <v>1091</v>
+      </c>
+      <c r="M1548" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="N1548" s="4">
+        <v>3.4</v>
+      </c>
+      <c r="O1548" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1548" s="3"/>
+      <c r="Q1548" s="2"/>
+    </row>
+    <row r="1549" spans="10:17" ht="15.75" thickBot="1">
+      <c r="J1549" s="2" t="s">
+        <v>1092</v>
+      </c>
+      <c r="K1549" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1549" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="M1549" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="N1549" s="4">
+        <v>1</v>
+      </c>
+      <c r="O1549" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1549" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="Q1549" s="2"/>
+    </row>
+    <row r="1550" spans="10:17" ht="15.75" thickBot="1">
+      <c r="J1550" s="2" t="s">
+        <v>1093</v>
+      </c>
+      <c r="K1550" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1550" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="M1550" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="N1550" s="4">
+        <v>2</v>
+      </c>
+      <c r="O1550" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1550" s="3"/>
+      <c r="Q1550" s="2"/>
+    </row>
+    <row r="1551" spans="10:17" ht="15.75" thickBot="1">
+      <c r="J1551" s="2" t="s">
+        <v>1094</v>
+      </c>
+      <c r="K1551" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1551" s="2" t="s">
+        <v>1095</v>
+      </c>
+      <c r="M1551" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="N1551" s="4">
+        <v>1</v>
+      </c>
+      <c r="O1551" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1551" s="3">
+        <v>-0.35</v>
+      </c>
+      <c r="Q1551" s="2"/>
+    </row>
+    <row r="1552" spans="10:17" ht="15.75" thickBot="1">
+      <c r="J1552" s="2" t="s">
+        <v>1096</v>
+      </c>
+      <c r="K1552" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1552" s="2" t="s">
+        <v>1095</v>
+      </c>
+      <c r="M1552" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="N1552" s="4">
+        <v>2.85</v>
+      </c>
+      <c r="O1552" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1552" s="3"/>
+      <c r="Q1552" s="2"/>
+    </row>
+    <row r="1553" spans="10:17" ht="15.75" thickBot="1">
+      <c r="J1553" s="2" t="s">
+        <v>1097</v>
+      </c>
+      <c r="K1553" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1553" s="2" t="s">
+        <v>1098</v>
+      </c>
+      <c r="M1553" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="N1553" s="4">
+        <v>4.55</v>
+      </c>
+      <c r="O1553" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="P1553" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="Q1553" s="2"/>
+    </row>
+    <row r="1554" spans="10:17" ht="15.75" thickBot="1">
+      <c r="J1554" s="2" t="s">
+        <v>1099</v>
+      </c>
+      <c r="K1554" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1554" s="2" t="s">
+        <v>1098</v>
+      </c>
+      <c r="M1554" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="N1554" s="4">
+        <v>3.05</v>
+      </c>
+      <c r="O1554" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1554" s="3"/>
+      <c r="Q1554" s="2"/>
+    </row>
+    <row r="1555" spans="10:17" ht="15.75" thickBot="1">
+      <c r="J1555" s="2" t="s">
+        <v>1100</v>
+      </c>
+      <c r="K1555" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1555" s="2" t="s">
+        <v>1101</v>
+      </c>
+      <c r="M1555" s="3">
         <v>-0.2</v>
       </c>
-      <c r="N1486" s="4">
-        <v>3.25</v>
-      </c>
-      <c r="O1486" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="P1486" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="Q1486" s="2"/>
-    </row>
-    <row r="1487" spans="1:17" ht="15.75" thickBot="1">
-      <c r="J1487" s="2" t="s">
-        <v>1050</v>
-      </c>
-      <c r="K1487" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1487" s="2" t="s">
-        <v>1049</v>
-      </c>
-      <c r="M1487" s="5">
+      <c r="N1555" s="4">
+        <v>2</v>
+      </c>
+      <c r="O1555" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1555" s="3">
+        <v>-0.16</v>
+      </c>
+      <c r="Q1555" s="2"/>
+    </row>
+    <row r="1556" spans="10:17" ht="15.75" thickBot="1">
+      <c r="J1556" s="2" t="s">
+        <v>1102</v>
+      </c>
+      <c r="K1556" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1556" s="2" t="s">
+        <v>1101</v>
+      </c>
+      <c r="M1556" s="5">
         <v>0.2</v>
       </c>
-      <c r="N1487" s="4">
-        <v>2.75</v>
-      </c>
-      <c r="O1487" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1487" s="3"/>
-      <c r="Q1487" s="2"/>
-    </row>
-    <row r="1488" spans="1:17" ht="15.75" thickBot="1">
-      <c r="J1488" s="2" t="s">
-        <v>1051</v>
-      </c>
-      <c r="K1488" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1488" s="2" t="s">
-        <v>1052</v>
-      </c>
-      <c r="M1488" s="3">
-        <v>-0.5</v>
-      </c>
-      <c r="N1488" s="4">
-        <v>2</v>
-      </c>
-      <c r="O1488" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="P1488" s="3">
-        <v>-0.5</v>
-      </c>
-      <c r="Q1488" s="2"/>
-    </row>
-    <row r="1489" spans="10:17" ht="15.75" thickBot="1">
-      <c r="J1489" s="2" t="s">
-        <v>1053</v>
-      </c>
-      <c r="K1489" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1489" s="2" t="s">
-        <v>1052</v>
-      </c>
-      <c r="M1489" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="N1489" s="4">
-        <v>3</v>
-      </c>
-      <c r="O1489" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1489" s="3"/>
-      <c r="Q1489" s="2"/>
-    </row>
-    <row r="1490" spans="10:17" ht="15.75" thickBot="1">
-      <c r="J1490" s="2" t="s">
-        <v>1054</v>
-      </c>
-      <c r="K1490" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1490" s="2" t="s">
-        <v>1055</v>
-      </c>
-      <c r="M1490" s="3">
-        <v>-0.19</v>
-      </c>
-      <c r="N1490" s="4">
-        <v>2.25</v>
-      </c>
-      <c r="O1490" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="P1490" s="5">
-        <v>0.06</v>
-      </c>
-      <c r="Q1490" s="2"/>
-    </row>
-    <row r="1491" spans="10:17" ht="15.75" thickBot="1">
-      <c r="J1491" s="2" t="s">
-        <v>1056</v>
-      </c>
-      <c r="K1491" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1491" s="2" t="s">
-        <v>1055</v>
-      </c>
-      <c r="M1491" s="5">
-        <v>0.19</v>
-      </c>
-      <c r="N1491" s="4">
-        <v>1.95</v>
-      </c>
-      <c r="O1491" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1491" s="3"/>
-      <c r="Q1491" s="2"/>
-    </row>
-    <row r="1492" spans="10:17" ht="15.75" thickBot="1">
-      <c r="J1492" s="2" t="s">
-        <v>1057</v>
-      </c>
-      <c r="K1492" s="2" t="s">
-        <v>813</v>
-      </c>
-      <c r="L1492" s="2" t="s">
-        <v>1058</v>
-      </c>
-      <c r="M1492" s="3">
-        <v>-0.02</v>
-      </c>
-      <c r="N1492" s="4">
-        <v>27</v>
-      </c>
-      <c r="O1492" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="P1492" s="3">
-        <v>-0.84</v>
-      </c>
-      <c r="Q1492" s="2"/>
-    </row>
-    <row r="1493" spans="10:17" ht="15.75" thickBot="1">
-      <c r="J1493" s="2" t="s">
-        <v>1059</v>
-      </c>
-      <c r="K1493" s="2" t="s">
-        <v>813</v>
-      </c>
-      <c r="L1493" s="2" t="s">
-        <v>1058</v>
-      </c>
-      <c r="M1493" s="5">
-        <v>0.02</v>
-      </c>
-      <c r="N1493" s="4">
-        <v>69</v>
-      </c>
-      <c r="O1493" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1493" s="3"/>
-      <c r="Q1493" s="2"/>
-    </row>
-    <row r="1494" spans="10:17" ht="15.75" thickBot="1">
-      <c r="J1494" s="2" t="s">
-        <v>1060</v>
-      </c>
-      <c r="K1494" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="L1494" s="2" t="s">
-        <v>1061</v>
-      </c>
-      <c r="M1494" s="3">
-        <v>-0.01</v>
-      </c>
-      <c r="N1494" s="4">
-        <v>131</v>
-      </c>
-      <c r="O1494" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="P1494" s="5">
-        <v>0.23</v>
-      </c>
-      <c r="Q1494" s="2"/>
-    </row>
-    <row r="1495" spans="10:17" ht="15.75" thickBot="1">
-      <c r="J1495" s="2" t="s">
-        <v>1062</v>
-      </c>
-      <c r="K1495" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="L1495" s="2" t="s">
-        <v>1061</v>
-      </c>
-      <c r="M1495" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="N1495" s="4">
-        <v>108</v>
-      </c>
-      <c r="O1495" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1495" s="3"/>
-      <c r="Q1495" s="2"/>
-    </row>
-    <row r="1496" spans="10:17" ht="15.75" thickBot="1">
-      <c r="J1496" s="2" t="s">
-        <v>1063</v>
-      </c>
-      <c r="K1496" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="L1496" s="2" t="s">
-        <v>1064</v>
-      </c>
-      <c r="M1496" s="3">
-        <v>-0.01</v>
-      </c>
-      <c r="N1496" s="4">
-        <v>147</v>
-      </c>
-      <c r="O1496" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="P1496" s="5">
-        <v>0.35</v>
-      </c>
-      <c r="Q1496" s="2"/>
-    </row>
-    <row r="1497" spans="10:17" ht="15.75" thickBot="1">
-      <c r="J1497" s="2" t="s">
-        <v>1065</v>
-      </c>
-      <c r="K1497" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="L1497" s="2" t="s">
-        <v>1064</v>
-      </c>
-      <c r="M1497" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="N1497" s="4">
-        <v>112</v>
-      </c>
-      <c r="O1497" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1497" s="3"/>
-      <c r="Q1497" s="2"/>
-    </row>
-    <row r="1498" spans="10:17" ht="15.75" thickBot="1">
-      <c r="J1498" s="2" t="s">
-        <v>1066</v>
-      </c>
-      <c r="K1498" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="L1498" s="2" t="s">
-        <v>1067</v>
-      </c>
-      <c r="M1498" s="3">
-        <v>-0.05</v>
-      </c>
-      <c r="N1498" s="4">
-        <v>139</v>
-      </c>
-      <c r="O1498" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="P1498" s="5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Q1498" s="2"/>
-    </row>
-    <row r="1499" spans="10:17" ht="15.75" thickBot="1">
-      <c r="J1499" s="2" t="s">
-        <v>1068</v>
-      </c>
-      <c r="K1499" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1499" s="2" t="s">
-        <v>1069</v>
-      </c>
-      <c r="M1499" s="3">
-        <v>-0.5</v>
-      </c>
-      <c r="N1499" s="4">
-        <v>2.25</v>
-      </c>
-      <c r="O1499" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="P1499" s="5">
-        <v>0.13</v>
-      </c>
-      <c r="Q1499" s="2"/>
-    </row>
-    <row r="1500" spans="10:17" ht="15.75" thickBot="1">
-      <c r="J1500" s="2" t="s">
-        <v>1070</v>
-      </c>
-      <c r="K1500" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="L1500" s="2" t="s">
-        <v>1067</v>
-      </c>
-      <c r="M1500" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="N1500" s="4">
-        <v>117</v>
-      </c>
-      <c r="O1500" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1500" s="3"/>
-      <c r="Q1500" s="2"/>
-    </row>
-    <row r="1501" spans="10:17" ht="15.75" thickBot="1">
-      <c r="J1501" s="2" t="s">
-        <v>1071</v>
-      </c>
-      <c r="K1501" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1501" s="2" t="s">
-        <v>1069</v>
-      </c>
-      <c r="M1501" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="N1501" s="4">
-        <v>2</v>
-      </c>
-      <c r="O1501" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1501" s="3"/>
-      <c r="Q1501" s="2"/>
-    </row>
-    <row r="1502" spans="10:17" ht="15.75" thickBot="1">
-      <c r="Q1502" s="2"/>
-    </row>
-    <row r="1503" spans="10:17" ht="15.75" thickBot="1">
-      <c r="Q1503" s="2"/>
-    </row>
-    <row r="1504" spans="10:17" ht="15.75" thickBot="1">
-      <c r="Q1504" s="2"/>
-    </row>
-    <row r="1505" spans="17:17" ht="15.75" thickBot="1">
-      <c r="Q1505" s="2"/>
-    </row>
-    <row r="1506" spans="17:17" ht="15.75" thickBot="1">
-      <c r="Q1506" s="2"/>
-    </row>
-    <row r="1507" spans="17:17">
-      <c r="Q1507" s="1"/>
+      <c r="N1556" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="O1556" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1556" s="3"/>
+      <c r="Q1556" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>